<commit_message>
fixed conditional formula issue
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="880" windowWidth="24840" windowHeight="19200"/>
+    <workbookView xWindow="7140" yWindow="460" windowWidth="24840" windowHeight="19200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Project_Name</t>
   </si>
@@ -184,13 +184,16 @@
   </si>
   <si>
     <t>Write_To_Editor</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,13 +221,6 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,17 +356,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -396,43 +386,17 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color theme="1"/>
@@ -484,246 +448,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
@@ -853,16 +577,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -977,31 +691,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A7:H29"/>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="40">
+    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="12">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="39">
+    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="11">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="38">
+    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="10">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Function_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="36">
+    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="9">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Function" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="35">
+    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="8">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="34">
+    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="7">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="33">
+    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="6">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="32">
+    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="5">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value3" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1305,8 +1019,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1377,259 +1091,256 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:D9 H8:H29">
-    <cfRule type="expression" dxfId="9" priority="14">
+  <conditionalFormatting sqref="D8:D29 H8:H29">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>OR($C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:F9 H8:H29 E10:F29">
-    <cfRule type="expression" dxfId="8" priority="16">
+  <conditionalFormatting sqref="D8:D29 H8:H29 E8:F29">
+    <cfRule type="expression" dxfId="3" priority="16">
       <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:E9 H8:H29 E10:E29">
-    <cfRule type="expression" dxfId="7" priority="15">
+  <conditionalFormatting sqref="D8:D29 H8:H29 E8:E29">
+    <cfRule type="expression" dxfId="2" priority="15">
       <formula>OR($C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Radio_Button",$C8="Select_Image",$C8="Select_Item",$C8="Select_Link")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H29">
-    <cfRule type="expression" dxfId="6" priority="13">
-      <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert")</formula>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:H8">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="D8:H29">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR($C8="Select_Dropdown")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7">
       <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22:C29">
-      <formula1>$C$3:$C$25</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1657,7 +1368,7 @@
           <x14:formula1>
             <xm:f>Lists!$C$3:$C$25</xm:f>
           </x14:formula1>
-          <xm:sqref>C8:C18</xm:sqref>
+          <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1668,10 +1379,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:C25"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1679,177 +1390,204 @@
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <sortState ref="C3:C23">

</xml_diff>

<commit_message>
added a browser quit function
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$25</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$26</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Project_Name</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Browser_Quit</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1023,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1360,13 +1363,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$10:$A$25</xm:f>
+            <xm:f>Lists!$A$10:$A$26</xm:f>
           </x14:formula1>
           <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$25</xm:f>
+            <xm:f>Lists!$C$3:$C$26</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1379,10 +1382,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:D25"/>
+  <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1436,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D6" s="21"/>
     </row>
@@ -1444,8 +1447,8 @@
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
+      <c r="C7" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -1453,8 +1456,8 @@
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
+      <c r="C8" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -1463,7 +1466,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -1472,7 +1475,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -1481,7 +1484,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -1490,7 +1493,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -1499,7 +1502,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4"/>
     </row>
@@ -1508,86 +1511,93 @@
         <v>17</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D26" s="4"/>
     </row>
   </sheetData>
   <sortState ref="C3:C23">

</xml_diff>

<commit_message>
added a new function to click on H_tag
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$26</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$27</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Project_Name</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Browser_Quit</t>
+  </si>
+  <si>
+    <t>Click_H_Tag</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1076,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1374,12 +1377,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D29 H8:H29 E8:E29">
-    <cfRule type="expression" dxfId="7" priority="15">
-      <formula>OR($C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Radio_Button",$C8="Select_Image",$C8="Select_Item",$C8="Select_Link")</formula>
+    <cfRule type="expression" dxfId="5" priority="15">
+      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Radio_Button",$C8="Select_Image",$C8="Select_Item",$C8="Select_Link")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H29">
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login",$C8="Browser_Quit")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1413,13 +1416,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$10:$A$26</xm:f>
+            <xm:f>Lists!$A$10:$A$27</xm:f>
           </x14:formula1>
           <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$26</xm:f>
+            <xm:f>Lists!$C$3:$C$27</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1432,10 +1435,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:D26"/>
+  <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1568,86 +1571,93 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="C27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <sortState ref="C3:C23">

</xml_diff>

<commit_message>
updated to allow user to skip indiviual test cases
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/GitHub/TAF/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/QA_Tools/taf/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="460" windowWidth="24840" windowHeight="19200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30020" windowHeight="19200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$27</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$34</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Project_Name</t>
   </si>
@@ -186,13 +186,55 @@
     <t>Write_To_Editor</t>
   </si>
   <si>
+    <t>Portal_Login</t>
+  </si>
+  <si>
+    <t>Admin_Portal_Login</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>Custom Function to login to portal</t>
+  </si>
+  <si>
+    <t>Custom Function to login to Admin portal</t>
+  </si>
+  <si>
+    <t>Custom for Portal but may work with others</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
     <t>Browser_Quit</t>
   </si>
   <si>
+    <t>Open_Portal_URL</t>
+  </si>
+  <si>
+    <t>Custom for Portal</t>
+  </si>
+  <si>
     <t>Click_H_Tag</t>
+  </si>
+  <si>
+    <t>Insert_value_config</t>
+  </si>
+  <si>
+    <t>Handle_Browser_Window</t>
+  </si>
+  <si>
+    <t>SINT_Login</t>
+  </si>
+  <si>
+    <t>Custom Function to login to sint</t>
+  </si>
+  <si>
+    <t>Send_Special_Keys</t>
+  </si>
+  <si>
+    <t>Skip_Test_Case</t>
   </si>
 </sst>
 </file>
@@ -232,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +305,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -335,13 +383,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -392,66 +455,49 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="16">
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -535,8 +581,8 @@
           <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -549,6 +595,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -747,33 +795,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A7:H29"/>
-  <tableColumns count="8">
-    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:I29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A7:I29"/>
+  <tableColumns count="9">
+    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="13">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="16">
+    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="12">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="15">
+    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="11">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Function_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="14">
+    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="10">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Function" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="13">
+    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="9">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="12">
+    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="8">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="11">
+    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="7">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="10">
+    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="6">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value3" xmlDataType="string"/>
     </tableColumn>
+    <tableColumn id="8" uniqueName="8" name="Skip_Test_Case" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1073,10 +1122,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1089,9 +1138,10 @@
     <col min="6" max="6" width="26.5" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1102,12 +1152,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1115,11 +1165,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1144,8 +1194,11 @@
       <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
@@ -1154,88 +1207,97 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="15"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="15"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="15"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9"/>
@@ -1244,8 +1306,9 @@
       <c r="F17" s="18"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
@@ -1254,8 +1317,9 @@
       <c r="F18" s="18"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="11"/>
       <c r="C19" s="9"/>
@@ -1264,8 +1328,9 @@
       <c r="F19" s="18"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
@@ -1274,8 +1339,9 @@
       <c r="F20" s="18"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
@@ -1284,8 +1350,9 @@
       <c r="F21" s="19"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
@@ -1294,8 +1361,9 @@
       <c r="F22" s="18"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
@@ -1304,8 +1372,9 @@
       <c r="F23" s="18"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
@@ -1314,8 +1383,9 @@
       <c r="F24" s="18"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
@@ -1324,8 +1394,9 @@
       <c r="F25" s="18"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
@@ -1334,8 +1405,9 @@
       <c r="F26" s="18"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
@@ -1344,8 +1416,9 @@
       <c r="F27" s="18"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
@@ -1354,8 +1427,9 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="11"/>
       <c r="C29" s="9"/>
@@ -1364,39 +1438,43 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
+      <c r="I29" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:D29 H8:H29">
-    <cfRule type="expression" dxfId="9" priority="14">
-      <formula>OR($C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title")</formula>
+  <conditionalFormatting sqref="D8:D29 H8:I29">
+    <cfRule type="expression" dxfId="5" priority="16">
+      <formula>OR($C8="Handle_Browser_window",$C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title",$C8="Open_Portal_URL",$C8="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D29 H8:H29 E8:F29">
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data")</formula>
+  <conditionalFormatting sqref="D8:F29 H8:I29">
+    <cfRule type="expression" dxfId="4" priority="18">
+      <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data",$C8="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D29 H8:H29 E8:E29">
-    <cfRule type="expression" dxfId="6" priority="15">
+  <conditionalFormatting sqref="D8:E29 H8:I29">
+    <cfRule type="expression" dxfId="3" priority="17">
       <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Select_Image",$C8="Select_Item",$C8="Select_Link")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H29">
-    <cfRule type="expression" dxfId="7" priority="13">
-      <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login",$C8="Browser_Quit")</formula>
+  <conditionalFormatting sqref="H8:I29">
+    <cfRule type="expression" dxfId="2" priority="15">
+      <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login",$C8="Browser_Quit",$C8="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:H29">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="D8:I29">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>OR($C8="Select_Dropdown",$C8="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7">
       <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:I29">
+      <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1410,19 +1488,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$3:$A$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>G8:G29 E8:E29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$A$10:$A$27</xm:f>
+            <xm:f>Lists!$A$10:$A$33</xm:f>
           </x14:formula1>
           <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$27</xm:f>
+            <xm:f>Lists!$A$3:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E29 G8:G29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$C$3:$C$34</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1435,17 +1513,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:D27"/>
+  <dimension ref="A2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" customWidth="1"/>
     <col min="4" max="4" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1457,7 +1535,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1480,7 +1558,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>42</v>
@@ -1489,25 +1567,27 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="21"/>
+        <v>34</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>48</v>
@@ -1516,7 +1596,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>13</v>
@@ -1525,7 +1605,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>15</v>
@@ -1534,7 +1614,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>41</v>
@@ -1543,7 +1623,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>18</v>
@@ -1552,7 +1632,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -1561,7 +1641,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>20</v>
@@ -1569,95 +1649,155 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" s="8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="C18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="C18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="C22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="C22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="C28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="C30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="C31" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="C32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="C33" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="C3:C23">
@@ -1670,6 +1810,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1678,7 +1824,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008EB026D4FC24C9499CD13E6F13776440" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bde19c557e1184fdfae2ef1e0c5f05ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1792,13 +1938,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCFE370-73EB-49D2-AC8E-6E5DA8D680F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25912E3-2FE1-4D2E-9563-62B2AC5168D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1806,7 +1961,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5F1915-B19E-426D-A8AF-460F08801EF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1820,19 +1975,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCFE370-73EB-49D2-AC8E-6E5DA8D680F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed select_Itam function as the click_button function has been updated to support this
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/QA_Tools/taf/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/GitHub/TAF/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30020" windowHeight="19200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$34</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$29</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Project_Name</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Browser_Forward</t>
   </si>
   <si>
-    <t>Select_Item</t>
-  </si>
-  <si>
     <t>Capture_Alert</t>
   </si>
   <si>
@@ -186,21 +183,9 @@
     <t>Write_To_Editor</t>
   </si>
   <si>
-    <t>Portal_Login</t>
-  </si>
-  <si>
-    <t>Admin_Portal_Login</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Custom Function to login to portal</t>
-  </si>
-  <si>
-    <t>Custom Function to login to Admin portal</t>
-  </si>
-  <si>
     <t>Custom for Portal but may work with others</t>
   </si>
   <si>
@@ -210,12 +195,6 @@
     <t>Browser_Quit</t>
   </si>
   <si>
-    <t>Open_Portal_URL</t>
-  </si>
-  <si>
-    <t>Custom for Portal</t>
-  </si>
-  <si>
     <t>Click_H_Tag</t>
   </si>
   <si>
@@ -223,12 +202,6 @@
   </si>
   <si>
     <t>Handle_Browser_Window</t>
-  </si>
-  <si>
-    <t>SINT_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to sint</t>
   </si>
   <si>
     <t>Send_Special_Keys</t>
@@ -476,30 +449,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -548,6 +497,30 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -822,7 +795,7 @@
     <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="6">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="8" name="Skip_Test_Case" dataDxfId="0"/>
+    <tableColumn id="8" uniqueName="8" name="Skip_Test_Case" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1124,8 +1097,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1442,27 +1415,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D29 H8:I29">
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="4" priority="16">
       <formula>OR($C8="Handle_Browser_window",$C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title",$C8="Open_Portal_URL",$C8="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:F29 H8:I29">
-    <cfRule type="expression" dxfId="4" priority="18">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data",$C8="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E29 H8:I29">
-    <cfRule type="expression" dxfId="3" priority="17">
-      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Select_Image",$C8="Select_Item",$C8="Select_Link")</formula>
+    <cfRule type="expression" dxfId="2" priority="17">
+      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Select_Image",$C8="Select_Link")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:I29">
-    <cfRule type="expression" dxfId="2" priority="15">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login",$C8="Browser_Quit",$C8="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:I29">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>OR($C8="Select_Dropdown",$C8="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1488,19 +1461,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$10:$A$33</xm:f>
-          </x14:formula1>
-          <xm:sqref>G7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Lists!$A$3:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>E8:E29 G8:G29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$34</xm:f>
+            <xm:f>Lists!$A$10:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>G7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$C$3:$C$29</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1513,10 +1486,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:D34"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1508,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1558,7 +1531,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>42</v>
@@ -1570,7 +1543,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D6" s="23"/>
     </row>
@@ -1579,10 +1552,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1590,7 +1563,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -1653,14 +1626,14 @@
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -1674,10 +1647,10 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1703,101 +1676,59 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="C22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>59</v>
-      </c>
+      <c r="C22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="C30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="C31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="C32" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="C33" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="C3:C23">

</xml_diff>

<commit_message>
removed functions select_image and Select_link as they are now covered in Click_button function
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$29</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$27</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Project_Name</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Select_Dropdown</t>
   </si>
   <si>
-    <t>Select_Link</t>
-  </si>
-  <si>
     <t>Write_Box_Data</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
   </si>
   <si>
     <t>Capture_Alert</t>
-  </si>
-  <si>
-    <t>Select_Image</t>
   </si>
   <si>
     <t>Check_Browser_Title</t>
@@ -447,7 +441,57 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -768,34 +812,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:I29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:I29" tableType="xml" insertRowShift="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A7:I29"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="13">
+    <tableColumn id="1" uniqueName="Test_Step" name="Test_Step" dataDxfId="18">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="12">
+    <tableColumn id="2" uniqueName="Test_Step_Description" name="Test_Step_Description" dataDxfId="17">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="11">
+    <tableColumn id="3" uniqueName="Test_Function_Type" name="Test_Step_Function" dataDxfId="16">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Function_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="10">
+    <tableColumn id="4" uniqueName="Test_Step_Function" name="Test_Step_Value" dataDxfId="15">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Function" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="9">
+    <tableColumn id="5" uniqueName="Test_Step_Value" name="Locator_Finder_Value" dataDxfId="14">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="8">
+    <tableColumn id="6" uniqueName="Locator_Finder_Value" name="Test_Step_Value2" dataDxfId="13">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="7">
+    <tableColumn id="7" uniqueName="Test_Step_Value2" name="Locator_Finder_Value2" dataDxfId="12">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Test_Step_Value2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="6">
+    <tableColumn id="10" uniqueName="Locator_Finder_Value3" name="Screenshot" dataDxfId="11">
       <xmlColumnPr mapId="2" xpath="/Test_Automation/Test_Case_Rows/Test_Case_Row/Locator_Finder_Value3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="8" name="Skip_Test_Case" dataDxfId="5"/>
+    <tableColumn id="8" uniqueName="8" name="Skip_Test_Case" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1097,8 +1141,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1415,27 +1459,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D29 H8:I29">
-    <cfRule type="expression" dxfId="4" priority="16">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>OR($C8="Handle_Browser_window",$C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title",$C8="Open_Portal_URL",$C8="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:F29 H8:I29">
-    <cfRule type="expression" dxfId="3" priority="18">
+    <cfRule type="expression" dxfId="8" priority="18">
       <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data",$C8="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E29 H8:I29">
-    <cfRule type="expression" dxfId="2" priority="17">
-      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values",$C8="Select_Image",$C8="Select_Link")</formula>
+    <cfRule type="expression" dxfId="5" priority="17">
+      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:I29">
-    <cfRule type="expression" dxfId="1" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Portal_Login",$C8="Admin_Portal_Login",$C8="Browser_Quit",$C8="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:I29">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>OR($C8="Select_Dropdown",$C8="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1467,13 +1511,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$10:$A$29</xm:f>
+            <xm:f>Lists!$A$10:$A$27</xm:f>
           </x14:formula1>
           <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$29</xm:f>
+            <xm:f>Lists!$C$3:$C$27</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1486,10 +1530,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:D29"/>
+  <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1502,48 +1546,48 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="23"/>
     </row>
@@ -1552,24 +1596,24 @@
         <v>14</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>13</v>
@@ -1587,16 +1631,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>18</v>
@@ -1605,7 +1649,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -1614,7 +1658,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>20</v>
@@ -1626,37 +1670,37 @@
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="4"/>
     </row>
@@ -1677,14 +1721,14 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="4"/>
     </row>
@@ -1698,7 +1742,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D25" s="4"/>
     </row>
@@ -1712,23 +1756,9 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="C28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="C29" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="4"/>
     </row>
   </sheetData>
   <sortState ref="C3:C23">
@@ -1741,21 +1771,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008EB026D4FC24C9499CD13E6F13776440" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bde19c557e1184fdfae2ef1e0c5f05ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1869,7 +1884,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5F1915-B19E-426D-A8AF-460F08801EF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCFE370-73EB-49D2-AC8E-6E5DA8D680F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1884,26 +1930,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25912E3-2FE1-4D2E-9563-62B2AC5168D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5F1915-B19E-426D-A8AF-460F08801EF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removed result_file,puts from code and removed click_h_tag from code and spread sheet, Updating the new click_button function
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -19,7 +19,7 @@
     <definedName name="Broker_Functions">Lists!#REF!</definedName>
     <definedName name="GUI_Functions">Lists!#REF!</definedName>
     <definedName name="NiFi_Functions">Lists!#REF!</definedName>
-    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$27</definedName>
+    <definedName name="Ruby_Web_Functions">Lists!$C$5:$C$26</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Project_Name</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Browser_Quit</t>
-  </si>
-  <si>
-    <t>Click_H_Tag</t>
   </si>
   <si>
     <t>Insert_value_config</t>
@@ -1142,7 +1139,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1212,7 +1209,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1470,7 +1467,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E29 H8:I29">
     <cfRule type="expression" dxfId="5" priority="17">
-      <formula>OR($C8="Click_H_Tag",$C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values")</formula>
+      <formula>OR($C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:I29">
@@ -1517,7 +1514,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$27</xm:f>
+            <xm:f>Lists!$C$3:$C$26</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C29</xm:sqref>
         </x14:dataValidation>
@@ -1533,7 +1530,7 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C15" sqref="C15:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1670,95 +1667,91 @@
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
-      <c r="C17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="C18" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>48</v>
-      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="C27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <sortState ref="C3:C23">
@@ -1771,6 +1764,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008EB026D4FC24C9499CD13E6F13776440" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bde19c557e1184fdfae2ef1e0c5f05ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1884,22 +1886,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25912E3-2FE1-4D2E-9563-62B2AC5168D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5F1915-B19E-426D-A8AF-460F08801EF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1915,7 +1916,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCFE370-73EB-49D2-AC8E-6E5DA8D680F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1928,12 +1929,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E25912E3-2FE1-4D2E-9563-62B2AC5168D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated spreadsheets to use autonumbering
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/GitHub/TAF/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/QA_Tools/taf/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="31080" windowHeight="18720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Spec" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Project_Name</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Custom Function to login to portal</t>
+  </si>
+  <si>
+    <t>SINT_Login</t>
+  </si>
+  <si>
+    <t>Custom Function to login to sint</t>
+  </si>
+  <si>
+    <t>Admin_Portal_Login</t>
+  </si>
+  <si>
+    <t>Custom Function to login to Admin portal</t>
   </si>
   <si>
     <t>Notes</t>
@@ -377,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,6 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,6 +448,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -872,21 +901,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1115,7 +1129,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Project_Name" dataDxfId="43"/>
     <tableColumn id="2" name="Project_ID" dataDxfId="42"/>
@@ -1127,58 +1140,58 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A7:I200" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="A7:I200"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Test_Step" dataDxfId="35"/>
-    <tableColumn id="2" name="Test_Step_Description" dataDxfId="34"/>
-    <tableColumn id="3" name="Test_Step_Function" dataDxfId="33"/>
-    <tableColumn id="4" name="Test_Step_Value" dataDxfId="32"/>
-    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="31"/>
-    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="30"/>
-    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="29"/>
-    <tableColumn id="8" name="Screenshot" dataDxfId="28"/>
-    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="27"/>
+    <tableColumn id="1" name="Test_Step" dataDxfId="0">
+      <calculatedColumnFormula>ROW(1:8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Test_Step_Description" dataDxfId="35"/>
+    <tableColumn id="3" name="Test_Step_Function" dataDxfId="34"/>
+    <tableColumn id="4" name="Test_Step_Value" dataDxfId="33"/>
+    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="32"/>
+    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="31"/>
+    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="30"/>
+    <tableColumn id="8" name="Screenshot" dataDxfId="29"/>
+    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:B5" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="A4:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:B5" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="2">
-    <tableColumn id="1" name="Test_ID" dataDxfId="22"/>
-    <tableColumn id="2" name="Test_Description" dataDxfId="21"/>
+    <tableColumn id="1" name="Test_ID" dataDxfId="23"/>
+    <tableColumn id="2" name="Test_Description" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A1:A27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:A29"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="15"/>
+    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="D1:D14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Locator" dataDxfId="9"/>
+    <tableColumn id="1" name="Ruby_Locator" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="B1:B27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B1:B29"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Notes" dataDxfId="5"/>
+    <tableColumn id="1" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1450,7 +1463,8 @@
   <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1507,2170 +1521,2749 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="1">
+        <f t="shared" ref="A8:A39" si="0">ROW(1:8)</f>
+        <v>1</v>
+      </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
+      <c r="A22" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
+      <c r="A23" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
+      <c r="A24" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
+      <c r="A25" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+      <c r="A28" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
+      <c r="A29" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
+      <c r="A30" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
+      <c r="A31" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+      <c r="A33" s="7">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+      <c r="A34" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="A35" s="7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="A36" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="A37" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="A38" s="7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+      <c r="A39" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
+      <c r="A40" s="7">
+        <f t="shared" ref="A40:A71" si="1">ROW(33:40)</f>
+        <v>33</v>
+      </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
+      <c r="A41" s="7">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
+      <c r="A42" s="7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
+      <c r="A43" s="7">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
+      <c r="A44" s="7">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
+      <c r="A45" s="7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
+      <c r="A46" s="7">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
+      <c r="A47" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
+      <c r="A48" s="7">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
+      <c r="A49" s="7">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
+      <c r="A50" s="7">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
+      <c r="A51" s="7">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
+      <c r="A52" s="7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
+      <c r="A56" s="7">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="7"/>
+      <c r="A57" s="7">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
+      <c r="A58" s="7">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="7"/>
+      <c r="A59" s="7">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="7"/>
+      <c r="A60" s="7">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="7"/>
+      <c r="A61" s="7">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="7"/>
+      <c r="A62" s="7">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="7"/>
+      <c r="A63" s="7">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="7"/>
+      <c r="A64" s="7">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
+      <c r="A65" s="7">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="7"/>
+      <c r="A66" s="7">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
+      <c r="A67" s="7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="7"/>
+      <c r="A68" s="7">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="7"/>
+      <c r="A69" s="7">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="7"/>
+      <c r="A70" s="7">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
+      <c r="A71" s="7">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="20"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="7"/>
+      <c r="A72" s="7">
+        <f t="shared" ref="A72:A103" si="2">ROW(65:72)</f>
+        <v>65</v>
+      </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="7"/>
+      <c r="A73" s="7">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="7"/>
+      <c r="A74" s="7">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="7"/>
+      <c r="A75" s="7">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="20"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="7"/>
+      <c r="A76" s="7">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="7"/>
+      <c r="A77" s="7">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="7"/>
+      <c r="A78" s="7">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="7"/>
+      <c r="A79" s="7">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="7"/>
+      <c r="A80" s="7">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="7"/>
+      <c r="A81" s="7">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="7"/>
+      <c r="A82" s="7">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="7"/>
+      <c r="A83" s="7">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="7"/>
+      <c r="A84" s="7">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="19"/>
-      <c r="H84" s="19"/>
-      <c r="I84" s="19"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="7"/>
+      <c r="A85" s="7">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
-      <c r="H85" s="19"/>
-      <c r="I85" s="19"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="7"/>
+      <c r="A86" s="7">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="19"/>
-      <c r="H86" s="19"/>
-      <c r="I86" s="19"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="7"/>
+      <c r="A87" s="7">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="19"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="19"/>
-      <c r="H87" s="19"/>
-      <c r="I87" s="19"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="20"/>
+      <c r="I87" s="20"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="7"/>
+      <c r="A88" s="7">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="20"/>
+      <c r="I88" s="20"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="7"/>
+      <c r="A89" s="7">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="19"/>
-      <c r="H89" s="19"/>
-      <c r="I89" s="19"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+      <c r="H89" s="20"/>
+      <c r="I89" s="20"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="7"/>
+      <c r="A90" s="7">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="7"/>
+      <c r="A91" s="7">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="19"/>
-      <c r="H91" s="19"/>
-      <c r="I91" s="19"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="20"/>
+      <c r="I91" s="20"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="7"/>
+      <c r="A92" s="7">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="19"/>
-      <c r="H92" s="19"/>
-      <c r="I92" s="19"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="20"/>
+      <c r="I92" s="20"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="7"/>
+      <c r="A93" s="7">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="19"/>
-      <c r="H93" s="19"/>
-      <c r="I93" s="19"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="7"/>
+      <c r="A94" s="7">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="19"/>
-      <c r="H94" s="19"/>
-      <c r="I94" s="19"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="20"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="7"/>
+      <c r="A95" s="7">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="19"/>
-      <c r="H95" s="19"/>
-      <c r="I95" s="19"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="7"/>
+      <c r="A96" s="7">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="19"/>
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="20"/>
+      <c r="I96" s="20"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="7"/>
+      <c r="A97" s="7">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="19"/>
-      <c r="H97" s="19"/>
-      <c r="I97" s="19"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="7"/>
+      <c r="A98" s="7">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
-      <c r="H98" s="19"/>
-      <c r="I98" s="19"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="20"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="7"/>
+      <c r="A99" s="7">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
-      <c r="F99" s="19"/>
-      <c r="G99" s="19"/>
-      <c r="H99" s="19"/>
-      <c r="I99" s="19"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="20"/>
+      <c r="H99" s="20"/>
+      <c r="I99" s="20"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="7"/>
+      <c r="A100" s="7">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
-      <c r="F100" s="19"/>
-      <c r="G100" s="19"/>
-      <c r="H100" s="19"/>
-      <c r="I100" s="19"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="20"/>
+      <c r="I100" s="20"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="7"/>
+      <c r="A101" s="7">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="19"/>
-      <c r="G101" s="19"/>
-      <c r="H101" s="19"/>
-      <c r="I101" s="19"/>
+      <c r="D101" s="20"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="20"/>
+      <c r="H101" s="20"/>
+      <c r="I101" s="20"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="7"/>
+      <c r="A102" s="7">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19"/>
-      <c r="F102" s="19"/>
-      <c r="G102" s="19"/>
-      <c r="H102" s="19"/>
-      <c r="I102" s="19"/>
+      <c r="D102" s="20"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
+      <c r="H102" s="20"/>
+      <c r="I102" s="20"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="7"/>
+      <c r="A103" s="7">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
-      <c r="G103" s="19"/>
-      <c r="H103" s="19"/>
-      <c r="I103" s="19"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="20"/>
+      <c r="I103" s="20"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A104" s="7"/>
+      <c r="A104" s="7">
+        <f t="shared" ref="A104:A135" si="3">ROW(97:104)</f>
+        <v>97</v>
+      </c>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="19"/>
-      <c r="F104" s="19"/>
-      <c r="G104" s="19"/>
-      <c r="H104" s="19"/>
-      <c r="I104" s="19"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="20"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="7"/>
+      <c r="A105" s="7">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="19"/>
-      <c r="H105" s="19"/>
-      <c r="I105" s="19"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A106" s="7"/>
+      <c r="A106" s="7">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="19"/>
-      <c r="H106" s="19"/>
-      <c r="I106" s="19"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
+      <c r="I106" s="20"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="7"/>
+      <c r="A107" s="7">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="19"/>
-      <c r="H107" s="19"/>
-      <c r="I107" s="19"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
+      <c r="I107" s="20"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="7"/>
+      <c r="A108" s="7">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="19"/>
-      <c r="H108" s="19"/>
-      <c r="I108" s="19"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+      <c r="I108" s="20"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7">
+        <f t="shared" si="3"/>
+        <v>102</v>
+      </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
-      <c r="D109" s="19"/>
-      <c r="E109" s="19"/>
-      <c r="F109" s="19"/>
-      <c r="G109" s="19"/>
-      <c r="H109" s="19"/>
-      <c r="I109" s="19"/>
+      <c r="D109" s="20"/>
+      <c r="E109" s="20"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20"/>
+      <c r="I109" s="20"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19"/>
-      <c r="H110" s="19"/>
-      <c r="I110" s="19"/>
+      <c r="D110" s="20"/>
+      <c r="E110" s="20"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="20"/>
+      <c r="I110" s="20"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="19"/>
-      <c r="H111" s="19"/>
-      <c r="I111" s="19"/>
+      <c r="D111" s="20"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" s="7"/>
+      <c r="A112" s="7">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="19"/>
-      <c r="H112" s="19"/>
-      <c r="I112" s="19"/>
+      <c r="D112" s="20"/>
+      <c r="E112" s="20"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="20"/>
+      <c r="I112" s="20"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="7"/>
+      <c r="A113" s="7">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="19"/>
-      <c r="H113" s="19"/>
-      <c r="I113" s="19"/>
+      <c r="D113" s="20"/>
+      <c r="E113" s="20"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+      <c r="I113" s="20"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="7"/>
+      <c r="A114" s="7">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="19"/>
-      <c r="H114" s="19"/>
-      <c r="I114" s="19"/>
+      <c r="D114" s="20"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+      <c r="I114" s="20"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="7"/>
+      <c r="A115" s="7">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
-      <c r="D115" s="19"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="19"/>
-      <c r="H115" s="19"/>
-      <c r="I115" s="19"/>
+      <c r="D115" s="20"/>
+      <c r="E115" s="20"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="20"/>
+      <c r="H115" s="20"/>
+      <c r="I115" s="20"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116" s="7"/>
+      <c r="A116" s="7">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="19"/>
-      <c r="H116" s="19"/>
-      <c r="I116" s="19"/>
+      <c r="D116" s="20"/>
+      <c r="E116" s="20"/>
+      <c r="F116" s="20"/>
+      <c r="G116" s="20"/>
+      <c r="H116" s="20"/>
+      <c r="I116" s="20"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="7"/>
+      <c r="A117" s="7">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
-      <c r="G117" s="19"/>
-      <c r="H117" s="19"/>
-      <c r="I117" s="19"/>
+      <c r="D117" s="20"/>
+      <c r="E117" s="20"/>
+      <c r="F117" s="20"/>
+      <c r="G117" s="20"/>
+      <c r="H117" s="20"/>
+      <c r="I117" s="20"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" s="7"/>
+      <c r="A118" s="7">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="19"/>
-      <c r="H118" s="19"/>
-      <c r="I118" s="19"/>
+      <c r="D118" s="20"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="20"/>
+      <c r="I118" s="20"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="7"/>
+      <c r="A119" s="7">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="19"/>
-      <c r="H119" s="19"/>
-      <c r="I119" s="19"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+      <c r="I119" s="20"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="7"/>
+      <c r="A120" s="7">
+        <f t="shared" si="3"/>
+        <v>113</v>
+      </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="19"/>
-      <c r="H120" s="19"/>
-      <c r="I120" s="19"/>
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
+      <c r="I120" s="20"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="7"/>
+      <c r="A121" s="7">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="19"/>
-      <c r="H121" s="19"/>
-      <c r="I121" s="19"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+      <c r="I121" s="20"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A122" s="7"/>
+      <c r="A122" s="7">
+        <f t="shared" si="3"/>
+        <v>115</v>
+      </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="19"/>
-      <c r="H122" s="19"/>
-      <c r="I122" s="19"/>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="20"/>
+      <c r="H122" s="20"/>
+      <c r="I122" s="20"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="7"/>
+      <c r="A123" s="7">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="19"/>
-      <c r="G123" s="19"/>
-      <c r="H123" s="19"/>
-      <c r="I123" s="19"/>
+      <c r="D123" s="20"/>
+      <c r="E123" s="20"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="20"/>
+      <c r="H123" s="20"/>
+      <c r="I123" s="20"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="7"/>
+      <c r="A124" s="7">
+        <f t="shared" si="3"/>
+        <v>117</v>
+      </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="19"/>
-      <c r="G124" s="19"/>
-      <c r="H124" s="19"/>
-      <c r="I124" s="19"/>
+      <c r="D124" s="20"/>
+      <c r="E124" s="20"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="20"/>
+      <c r="H124" s="20"/>
+      <c r="I124" s="20"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="7"/>
+      <c r="A125" s="7">
+        <f t="shared" si="3"/>
+        <v>118</v>
+      </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19"/>
-      <c r="F125" s="19"/>
-      <c r="G125" s="19"/>
-      <c r="H125" s="19"/>
-      <c r="I125" s="19"/>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+      <c r="F125" s="20"/>
+      <c r="G125" s="20"/>
+      <c r="H125" s="20"/>
+      <c r="I125" s="20"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="7"/>
+      <c r="A126" s="7">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
-      <c r="D126" s="19"/>
-      <c r="E126" s="19"/>
-      <c r="F126" s="19"/>
-      <c r="G126" s="19"/>
-      <c r="H126" s="19"/>
-      <c r="I126" s="19"/>
+      <c r="D126" s="20"/>
+      <c r="E126" s="20"/>
+      <c r="F126" s="20"/>
+      <c r="G126" s="20"/>
+      <c r="H126" s="20"/>
+      <c r="I126" s="20"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="7"/>
+      <c r="A127" s="7">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
-      <c r="D127" s="19"/>
-      <c r="E127" s="19"/>
-      <c r="F127" s="19"/>
-      <c r="G127" s="19"/>
-      <c r="H127" s="19"/>
-      <c r="I127" s="19"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="20"/>
+      <c r="H127" s="20"/>
+      <c r="I127" s="20"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="7"/>
+      <c r="A128" s="7">
+        <f t="shared" si="3"/>
+        <v>121</v>
+      </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="19"/>
-      <c r="G128" s="19"/>
-      <c r="H128" s="19"/>
-      <c r="I128" s="19"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
+      <c r="I128" s="20"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="7"/>
+      <c r="A129" s="7">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
-      <c r="D129" s="19"/>
-      <c r="E129" s="19"/>
-      <c r="F129" s="19"/>
-      <c r="G129" s="19"/>
-      <c r="H129" s="19"/>
-      <c r="I129" s="19"/>
+      <c r="D129" s="20"/>
+      <c r="E129" s="20"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="20"/>
+      <c r="H129" s="20"/>
+      <c r="I129" s="20"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="7"/>
+      <c r="A130" s="7">
+        <f t="shared" si="3"/>
+        <v>123</v>
+      </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19"/>
-      <c r="H130" s="19"/>
-      <c r="I130" s="19"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="20"/>
+      <c r="I130" s="20"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="7"/>
+      <c r="A131" s="7">
+        <f t="shared" si="3"/>
+        <v>124</v>
+      </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19"/>
-      <c r="F131" s="19"/>
-      <c r="G131" s="19"/>
-      <c r="H131" s="19"/>
-      <c r="I131" s="19"/>
+      <c r="D131" s="20"/>
+      <c r="E131" s="20"/>
+      <c r="F131" s="20"/>
+      <c r="G131" s="20"/>
+      <c r="H131" s="20"/>
+      <c r="I131" s="20"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="7"/>
+      <c r="A132" s="7">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="19"/>
-      <c r="F132" s="19"/>
-      <c r="G132" s="19"/>
-      <c r="H132" s="19"/>
-      <c r="I132" s="19"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="20"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="20"/>
+      <c r="H132" s="20"/>
+      <c r="I132" s="20"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" s="7"/>
+      <c r="A133" s="7">
+        <f t="shared" si="3"/>
+        <v>126</v>
+      </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
-      <c r="D133" s="19"/>
-      <c r="E133" s="19"/>
-      <c r="F133" s="19"/>
-      <c r="G133" s="19"/>
-      <c r="H133" s="19"/>
-      <c r="I133" s="19"/>
+      <c r="D133" s="20"/>
+      <c r="E133" s="20"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="20"/>
+      <c r="H133" s="20"/>
+      <c r="I133" s="20"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="7"/>
+      <c r="A134" s="7">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
-      <c r="D134" s="20"/>
-      <c r="E134" s="19"/>
-      <c r="F134" s="19"/>
-      <c r="G134" s="19"/>
-      <c r="H134" s="19"/>
-      <c r="I134" s="19"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="20"/>
+      <c r="F134" s="20"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="20"/>
+      <c r="I134" s="20"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="7"/>
+      <c r="A135" s="7">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
-      <c r="D135" s="20"/>
-      <c r="E135" s="19"/>
-      <c r="F135" s="19"/>
-      <c r="G135" s="19"/>
-      <c r="H135" s="19"/>
-      <c r="I135" s="19"/>
+      <c r="D135" s="21"/>
+      <c r="E135" s="20"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="20"/>
+      <c r="H135" s="20"/>
+      <c r="I135" s="20"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="7"/>
+      <c r="A136" s="7">
+        <f t="shared" ref="A136:A167" si="4">ROW(129:136)</f>
+        <v>129</v>
+      </c>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
-      <c r="D136" s="20"/>
-      <c r="E136" s="19"/>
-      <c r="F136" s="19"/>
-      <c r="G136" s="19"/>
-      <c r="H136" s="19"/>
-      <c r="I136" s="19"/>
+      <c r="D136" s="21"/>
+      <c r="E136" s="20"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="20"/>
+      <c r="H136" s="20"/>
+      <c r="I136" s="20"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="7"/>
+      <c r="A137" s="7">
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
-      <c r="D137" s="20"/>
-      <c r="E137" s="19"/>
-      <c r="F137" s="19"/>
-      <c r="G137" s="19"/>
-      <c r="H137" s="19"/>
-      <c r="I137" s="19"/>
+      <c r="D137" s="21"/>
+      <c r="E137" s="20"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="20"/>
+      <c r="H137" s="20"/>
+      <c r="I137" s="20"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="7"/>
+      <c r="A138" s="7">
+        <f t="shared" si="4"/>
+        <v>131</v>
+      </c>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
-      <c r="D138" s="20"/>
-      <c r="E138" s="19"/>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19"/>
-      <c r="H138" s="19"/>
-      <c r="I138" s="19"/>
+      <c r="D138" s="21"/>
+      <c r="E138" s="20"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="20"/>
+      <c r="H138" s="20"/>
+      <c r="I138" s="20"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139" s="7"/>
+      <c r="A139" s="7">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
-      <c r="D139" s="20"/>
-      <c r="E139" s="19"/>
-      <c r="F139" s="19"/>
-      <c r="G139" s="19"/>
-      <c r="H139" s="19"/>
-      <c r="I139" s="19"/>
+      <c r="D139" s="21"/>
+      <c r="E139" s="20"/>
+      <c r="F139" s="20"/>
+      <c r="G139" s="20"/>
+      <c r="H139" s="20"/>
+      <c r="I139" s="20"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A140" s="7"/>
+      <c r="A140" s="7">
+        <f t="shared" si="4"/>
+        <v>133</v>
+      </c>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="20"/>
-      <c r="E140" s="19"/>
-      <c r="F140" s="19"/>
-      <c r="G140" s="19"/>
-      <c r="H140" s="19"/>
-      <c r="I140" s="19"/>
+      <c r="D140" s="21"/>
+      <c r="E140" s="20"/>
+      <c r="F140" s="20"/>
+      <c r="G140" s="20"/>
+      <c r="H140" s="20"/>
+      <c r="I140" s="20"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="7"/>
+      <c r="A141" s="7">
+        <f t="shared" si="4"/>
+        <v>134</v>
+      </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
-      <c r="D141" s="20"/>
-      <c r="E141" s="19"/>
-      <c r="F141" s="19"/>
-      <c r="G141" s="19"/>
-      <c r="H141" s="19"/>
-      <c r="I141" s="19"/>
+      <c r="D141" s="21"/>
+      <c r="E141" s="20"/>
+      <c r="F141" s="20"/>
+      <c r="G141" s="20"/>
+      <c r="H141" s="20"/>
+      <c r="I141" s="20"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A142" s="7"/>
+      <c r="A142" s="7">
+        <f t="shared" si="4"/>
+        <v>135</v>
+      </c>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
-      <c r="D142" s="20"/>
-      <c r="E142" s="19"/>
-      <c r="F142" s="19"/>
-      <c r="G142" s="19"/>
-      <c r="H142" s="19"/>
-      <c r="I142" s="19"/>
+      <c r="D142" s="21"/>
+      <c r="E142" s="20"/>
+      <c r="F142" s="20"/>
+      <c r="G142" s="20"/>
+      <c r="H142" s="20"/>
+      <c r="I142" s="20"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="7"/>
+      <c r="A143" s="7">
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
-      <c r="D143" s="20"/>
-      <c r="E143" s="19"/>
-      <c r="F143" s="19"/>
-      <c r="G143" s="19"/>
-      <c r="H143" s="19"/>
-      <c r="I143" s="19"/>
+      <c r="D143" s="21"/>
+      <c r="E143" s="20"/>
+      <c r="F143" s="20"/>
+      <c r="G143" s="20"/>
+      <c r="H143" s="20"/>
+      <c r="I143" s="20"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A144" s="7"/>
+      <c r="A144" s="7">
+        <f t="shared" si="4"/>
+        <v>137</v>
+      </c>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
-      <c r="D144" s="20"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="19"/>
-      <c r="G144" s="19"/>
-      <c r="H144" s="19"/>
-      <c r="I144" s="19"/>
+      <c r="D144" s="21"/>
+      <c r="E144" s="20"/>
+      <c r="F144" s="20"/>
+      <c r="G144" s="20"/>
+      <c r="H144" s="20"/>
+      <c r="I144" s="20"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" s="7"/>
+      <c r="A145" s="7">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
-      <c r="D145" s="20"/>
-      <c r="E145" s="19"/>
-      <c r="F145" s="19"/>
-      <c r="G145" s="19"/>
-      <c r="H145" s="19"/>
-      <c r="I145" s="19"/>
+      <c r="D145" s="21"/>
+      <c r="E145" s="20"/>
+      <c r="F145" s="20"/>
+      <c r="G145" s="20"/>
+      <c r="H145" s="20"/>
+      <c r="I145" s="20"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" s="7"/>
+      <c r="A146" s="7">
+        <f t="shared" si="4"/>
+        <v>139</v>
+      </c>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
-      <c r="D146" s="20"/>
-      <c r="E146" s="19"/>
-      <c r="F146" s="19"/>
-      <c r="G146" s="19"/>
-      <c r="H146" s="19"/>
-      <c r="I146" s="19"/>
+      <c r="D146" s="21"/>
+      <c r="E146" s="20"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="20"/>
+      <c r="H146" s="20"/>
+      <c r="I146" s="20"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" s="7"/>
+      <c r="A147" s="7">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
-      <c r="D147" s="20"/>
-      <c r="E147" s="19"/>
-      <c r="F147" s="19"/>
-      <c r="G147" s="19"/>
-      <c r="H147" s="19"/>
-      <c r="I147" s="19"/>
+      <c r="D147" s="21"/>
+      <c r="E147" s="20"/>
+      <c r="F147" s="20"/>
+      <c r="G147" s="20"/>
+      <c r="H147" s="20"/>
+      <c r="I147" s="20"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A148" s="7"/>
+      <c r="A148" s="7">
+        <f t="shared" si="4"/>
+        <v>141</v>
+      </c>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
-      <c r="D148" s="20"/>
-      <c r="E148" s="19"/>
-      <c r="F148" s="19"/>
-      <c r="G148" s="19"/>
-      <c r="H148" s="19"/>
-      <c r="I148" s="19"/>
+      <c r="D148" s="21"/>
+      <c r="E148" s="20"/>
+      <c r="F148" s="20"/>
+      <c r="G148" s="20"/>
+      <c r="H148" s="20"/>
+      <c r="I148" s="20"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A149" s="7"/>
+      <c r="A149" s="7">
+        <f t="shared" si="4"/>
+        <v>142</v>
+      </c>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
-      <c r="D149" s="20"/>
-      <c r="E149" s="19"/>
-      <c r="F149" s="19"/>
-      <c r="G149" s="19"/>
-      <c r="H149" s="19"/>
-      <c r="I149" s="19"/>
+      <c r="D149" s="21"/>
+      <c r="E149" s="20"/>
+      <c r="F149" s="20"/>
+      <c r="G149" s="20"/>
+      <c r="H149" s="20"/>
+      <c r="I149" s="20"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A150" s="7"/>
+      <c r="A150" s="7">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
-      <c r="D150" s="20"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="19"/>
-      <c r="G150" s="19"/>
-      <c r="H150" s="19"/>
-      <c r="I150" s="19"/>
+      <c r="D150" s="21"/>
+      <c r="E150" s="20"/>
+      <c r="F150" s="20"/>
+      <c r="G150" s="20"/>
+      <c r="H150" s="20"/>
+      <c r="I150" s="20"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A151" s="7"/>
+      <c r="A151" s="7">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
-      <c r="D151" s="20"/>
-      <c r="E151" s="19"/>
-      <c r="F151" s="19"/>
-      <c r="G151" s="19"/>
-      <c r="H151" s="19"/>
-      <c r="I151" s="19"/>
+      <c r="D151" s="21"/>
+      <c r="E151" s="20"/>
+      <c r="F151" s="20"/>
+      <c r="G151" s="20"/>
+      <c r="H151" s="20"/>
+      <c r="I151" s="20"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A152" s="7"/>
+      <c r="A152" s="7">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
-      <c r="D152" s="20"/>
-      <c r="E152" s="19"/>
-      <c r="F152" s="19"/>
-      <c r="G152" s="19"/>
-      <c r="H152" s="19"/>
-      <c r="I152" s="19"/>
+      <c r="D152" s="21"/>
+      <c r="E152" s="20"/>
+      <c r="F152" s="20"/>
+      <c r="G152" s="20"/>
+      <c r="H152" s="20"/>
+      <c r="I152" s="20"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A153" s="7"/>
+      <c r="A153" s="7">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="19"/>
-      <c r="G153" s="19"/>
-      <c r="H153" s="19"/>
-      <c r="I153" s="19"/>
+      <c r="D153" s="20"/>
+      <c r="E153" s="20"/>
+      <c r="F153" s="20"/>
+      <c r="G153" s="20"/>
+      <c r="H153" s="20"/>
+      <c r="I153" s="20"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="7"/>
+      <c r="A154" s="7">
+        <f t="shared" si="4"/>
+        <v>147</v>
+      </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="19"/>
-      <c r="G154" s="19"/>
-      <c r="H154" s="19"/>
-      <c r="I154" s="19"/>
+      <c r="D154" s="20"/>
+      <c r="E154" s="20"/>
+      <c r="F154" s="20"/>
+      <c r="G154" s="20"/>
+      <c r="H154" s="20"/>
+      <c r="I154" s="20"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A155" s="7"/>
+      <c r="A155" s="7">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
-      <c r="D155" s="19"/>
-      <c r="E155" s="19"/>
-      <c r="F155" s="19"/>
-      <c r="G155" s="19"/>
-      <c r="H155" s="19"/>
-      <c r="I155" s="19"/>
+      <c r="D155" s="20"/>
+      <c r="E155" s="20"/>
+      <c r="F155" s="20"/>
+      <c r="G155" s="20"/>
+      <c r="H155" s="20"/>
+      <c r="I155" s="20"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A156" s="7"/>
+      <c r="A156" s="7">
+        <f t="shared" si="4"/>
+        <v>149</v>
+      </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
-      <c r="D156" s="19"/>
-      <c r="E156" s="19"/>
-      <c r="F156" s="19"/>
-      <c r="G156" s="19"/>
-      <c r="H156" s="19"/>
-      <c r="I156" s="19"/>
+      <c r="D156" s="20"/>
+      <c r="E156" s="20"/>
+      <c r="F156" s="20"/>
+      <c r="G156" s="20"/>
+      <c r="H156" s="20"/>
+      <c r="I156" s="20"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A157" s="7"/>
+      <c r="A157" s="7">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="19"/>
-      <c r="G157" s="19"/>
-      <c r="H157" s="19"/>
-      <c r="I157" s="19"/>
+      <c r="D157" s="20"/>
+      <c r="E157" s="20"/>
+      <c r="F157" s="20"/>
+      <c r="G157" s="20"/>
+      <c r="H157" s="20"/>
+      <c r="I157" s="20"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A158" s="7"/>
+      <c r="A158" s="7">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
-      <c r="D158" s="19"/>
-      <c r="E158" s="19"/>
-      <c r="F158" s="19"/>
-      <c r="G158" s="19"/>
-      <c r="H158" s="19"/>
-      <c r="I158" s="19"/>
+      <c r="D158" s="20"/>
+      <c r="E158" s="20"/>
+      <c r="F158" s="20"/>
+      <c r="G158" s="20"/>
+      <c r="H158" s="20"/>
+      <c r="I158" s="20"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A159" s="7"/>
+      <c r="A159" s="7">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
-      <c r="D159" s="19"/>
-      <c r="E159" s="19"/>
-      <c r="F159" s="19"/>
-      <c r="G159" s="19"/>
-      <c r="H159" s="19"/>
-      <c r="I159" s="19"/>
+      <c r="D159" s="20"/>
+      <c r="E159" s="20"/>
+      <c r="F159" s="20"/>
+      <c r="G159" s="20"/>
+      <c r="H159" s="20"/>
+      <c r="I159" s="20"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A160" s="7"/>
+      <c r="A160" s="7">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
-      <c r="D160" s="19"/>
-      <c r="E160" s="19"/>
-      <c r="F160" s="19"/>
-      <c r="G160" s="19"/>
-      <c r="H160" s="19"/>
-      <c r="I160" s="19"/>
+      <c r="D160" s="20"/>
+      <c r="E160" s="20"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="20"/>
+      <c r="H160" s="20"/>
+      <c r="I160" s="20"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" s="7"/>
+      <c r="A161" s="7">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
-      <c r="D161" s="19"/>
-      <c r="E161" s="19"/>
-      <c r="F161" s="19"/>
-      <c r="G161" s="19"/>
-      <c r="H161" s="19"/>
-      <c r="I161" s="19"/>
+      <c r="D161" s="20"/>
+      <c r="E161" s="20"/>
+      <c r="F161" s="20"/>
+      <c r="G161" s="20"/>
+      <c r="H161" s="20"/>
+      <c r="I161" s="20"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" s="7"/>
+      <c r="A162" s="7">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
-      <c r="D162" s="19"/>
-      <c r="E162" s="19"/>
-      <c r="F162" s="19"/>
-      <c r="G162" s="19"/>
-      <c r="H162" s="19"/>
-      <c r="I162" s="19"/>
+      <c r="D162" s="20"/>
+      <c r="E162" s="20"/>
+      <c r="F162" s="20"/>
+      <c r="G162" s="20"/>
+      <c r="H162" s="20"/>
+      <c r="I162" s="20"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A163" s="7"/>
+      <c r="A163" s="7">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
-      <c r="D163" s="19"/>
-      <c r="E163" s="19"/>
-      <c r="F163" s="19"/>
-      <c r="G163" s="19"/>
-      <c r="H163" s="19"/>
-      <c r="I163" s="19"/>
+      <c r="D163" s="20"/>
+      <c r="E163" s="20"/>
+      <c r="F163" s="20"/>
+      <c r="G163" s="20"/>
+      <c r="H163" s="20"/>
+      <c r="I163" s="20"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A164" s="7"/>
+      <c r="A164" s="7">
+        <f t="shared" si="4"/>
+        <v>157</v>
+      </c>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
-      <c r="D164" s="19"/>
-      <c r="E164" s="19"/>
-      <c r="F164" s="19"/>
-      <c r="G164" s="19"/>
-      <c r="H164" s="19"/>
-      <c r="I164" s="19"/>
+      <c r="D164" s="20"/>
+      <c r="E164" s="20"/>
+      <c r="F164" s="20"/>
+      <c r="G164" s="20"/>
+      <c r="H164" s="20"/>
+      <c r="I164" s="20"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
-      <c r="D165" s="19"/>
-      <c r="E165" s="19"/>
-      <c r="F165" s="19"/>
-      <c r="G165" s="19"/>
-      <c r="H165" s="19"/>
-      <c r="I165" s="19"/>
+      <c r="D165" s="20"/>
+      <c r="E165" s="20"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="20"/>
+      <c r="H165" s="20"/>
+      <c r="I165" s="20"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7">
+        <f t="shared" si="4"/>
+        <v>159</v>
+      </c>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
-      <c r="D166" s="19"/>
-      <c r="E166" s="19"/>
-      <c r="F166" s="19"/>
-      <c r="G166" s="19"/>
-      <c r="H166" s="19"/>
-      <c r="I166" s="19"/>
+      <c r="D166" s="20"/>
+      <c r="E166" s="20"/>
+      <c r="F166" s="20"/>
+      <c r="G166" s="20"/>
+      <c r="H166" s="20"/>
+      <c r="I166" s="20"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
-      <c r="D167" s="19"/>
-      <c r="E167" s="19"/>
-      <c r="F167" s="19"/>
-      <c r="G167" s="19"/>
-      <c r="H167" s="19"/>
-      <c r="I167" s="19"/>
+      <c r="D167" s="20"/>
+      <c r="E167" s="20"/>
+      <c r="F167" s="20"/>
+      <c r="G167" s="20"/>
+      <c r="H167" s="20"/>
+      <c r="I167" s="20"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A168" s="7"/>
+      <c r="A168" s="7">
+        <f t="shared" ref="A168:A199" si="5">ROW(161:168)</f>
+        <v>161</v>
+      </c>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
-      <c r="D168" s="19"/>
-      <c r="E168" s="19"/>
-      <c r="F168" s="19"/>
-      <c r="G168" s="19"/>
-      <c r="H168" s="19"/>
-      <c r="I168" s="19"/>
+      <c r="D168" s="20"/>
+      <c r="E168" s="20"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="20"/>
+      <c r="H168" s="20"/>
+      <c r="I168" s="20"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A169" s="7"/>
+      <c r="A169" s="7">
+        <f t="shared" si="5"/>
+        <v>162</v>
+      </c>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
-      <c r="D169" s="19"/>
-      <c r="E169" s="19"/>
-      <c r="F169" s="19"/>
-      <c r="G169" s="19"/>
-      <c r="H169" s="19"/>
-      <c r="I169" s="19"/>
+      <c r="D169" s="20"/>
+      <c r="E169" s="20"/>
+      <c r="F169" s="20"/>
+      <c r="G169" s="20"/>
+      <c r="H169" s="20"/>
+      <c r="I169" s="20"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A170" s="7"/>
+      <c r="A170" s="7">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
-      <c r="D170" s="19"/>
-      <c r="E170" s="19"/>
-      <c r="F170" s="19"/>
-      <c r="G170" s="19"/>
-      <c r="H170" s="19"/>
-      <c r="I170" s="19"/>
+      <c r="D170" s="20"/>
+      <c r="E170" s="20"/>
+      <c r="F170" s="20"/>
+      <c r="G170" s="20"/>
+      <c r="H170" s="20"/>
+      <c r="I170" s="20"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" s="7"/>
+      <c r="A171" s="7">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
-      <c r="D171" s="19"/>
-      <c r="E171" s="19"/>
-      <c r="F171" s="19"/>
-      <c r="G171" s="19"/>
-      <c r="H171" s="19"/>
-      <c r="I171" s="19"/>
+      <c r="D171" s="20"/>
+      <c r="E171" s="20"/>
+      <c r="F171" s="20"/>
+      <c r="G171" s="20"/>
+      <c r="H171" s="20"/>
+      <c r="I171" s="20"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A172" s="7"/>
+      <c r="A172" s="7">
+        <f t="shared" si="5"/>
+        <v>165</v>
+      </c>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
-      <c r="D172" s="19"/>
-      <c r="E172" s="19"/>
-      <c r="F172" s="19"/>
-      <c r="G172" s="19"/>
-      <c r="H172" s="19"/>
-      <c r="I172" s="19"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="20"/>
+      <c r="F172" s="20"/>
+      <c r="G172" s="20"/>
+      <c r="H172" s="20"/>
+      <c r="I172" s="20"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A173" s="7"/>
+      <c r="A173" s="7">
+        <f t="shared" si="5"/>
+        <v>166</v>
+      </c>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
-      <c r="D173" s="19"/>
-      <c r="E173" s="19"/>
-      <c r="F173" s="19"/>
-      <c r="G173" s="19"/>
-      <c r="H173" s="19"/>
-      <c r="I173" s="19"/>
+      <c r="D173" s="20"/>
+      <c r="E173" s="20"/>
+      <c r="F173" s="20"/>
+      <c r="G173" s="20"/>
+      <c r="H173" s="20"/>
+      <c r="I173" s="20"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A174" s="7"/>
+      <c r="A174" s="7">
+        <f t="shared" si="5"/>
+        <v>167</v>
+      </c>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
-      <c r="D174" s="19"/>
-      <c r="E174" s="19"/>
-      <c r="F174" s="19"/>
-      <c r="G174" s="19"/>
-      <c r="H174" s="19"/>
-      <c r="I174" s="19"/>
+      <c r="D174" s="20"/>
+      <c r="E174" s="20"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="20"/>
+      <c r="H174" s="20"/>
+      <c r="I174" s="20"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A175" s="7"/>
+      <c r="A175" s="7">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
-      <c r="D175" s="20"/>
-      <c r="E175" s="19"/>
-      <c r="F175" s="19"/>
-      <c r="G175" s="19"/>
-      <c r="H175" s="19"/>
-      <c r="I175" s="19"/>
+      <c r="D175" s="21"/>
+      <c r="E175" s="20"/>
+      <c r="F175" s="20"/>
+      <c r="G175" s="20"/>
+      <c r="H175" s="20"/>
+      <c r="I175" s="20"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A176" s="7"/>
+      <c r="A176" s="7">
+        <f t="shared" si="5"/>
+        <v>169</v>
+      </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
-      <c r="D176" s="20"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="19"/>
-      <c r="G176" s="19"/>
-      <c r="H176" s="19"/>
-      <c r="I176" s="19"/>
+      <c r="D176" s="21"/>
+      <c r="E176" s="20"/>
+      <c r="F176" s="20"/>
+      <c r="G176" s="20"/>
+      <c r="H176" s="20"/>
+      <c r="I176" s="20"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A177" s="7"/>
+      <c r="A177" s="7">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="20"/>
-      <c r="E177" s="19"/>
-      <c r="F177" s="19"/>
-      <c r="G177" s="19"/>
-      <c r="H177" s="19"/>
-      <c r="I177" s="19"/>
+      <c r="D177" s="21"/>
+      <c r="E177" s="20"/>
+      <c r="F177" s="20"/>
+      <c r="G177" s="20"/>
+      <c r="H177" s="20"/>
+      <c r="I177" s="20"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A178" s="7"/>
+      <c r="A178" s="7">
+        <f t="shared" si="5"/>
+        <v>171</v>
+      </c>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="20"/>
-      <c r="E178" s="19"/>
-      <c r="F178" s="19"/>
-      <c r="G178" s="19"/>
-      <c r="H178" s="19"/>
-      <c r="I178" s="19"/>
+      <c r="D178" s="21"/>
+      <c r="E178" s="20"/>
+      <c r="F178" s="20"/>
+      <c r="G178" s="20"/>
+      <c r="H178" s="20"/>
+      <c r="I178" s="20"/>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A179" s="7"/>
+      <c r="A179" s="7">
+        <f t="shared" si="5"/>
+        <v>172</v>
+      </c>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
-      <c r="D179" s="20"/>
-      <c r="E179" s="19"/>
-      <c r="F179" s="19"/>
-      <c r="G179" s="19"/>
-      <c r="H179" s="19"/>
-      <c r="I179" s="19"/>
+      <c r="D179" s="21"/>
+      <c r="E179" s="20"/>
+      <c r="F179" s="20"/>
+      <c r="G179" s="20"/>
+      <c r="H179" s="20"/>
+      <c r="I179" s="20"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A180" s="7"/>
+      <c r="A180" s="7">
+        <f t="shared" si="5"/>
+        <v>173</v>
+      </c>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
-      <c r="D180" s="20"/>
-      <c r="E180" s="19"/>
-      <c r="F180" s="19"/>
-      <c r="G180" s="19"/>
-      <c r="H180" s="19"/>
-      <c r="I180" s="19"/>
+      <c r="D180" s="21"/>
+      <c r="E180" s="20"/>
+      <c r="F180" s="20"/>
+      <c r="G180" s="20"/>
+      <c r="H180" s="20"/>
+      <c r="I180" s="20"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A181" s="7"/>
+      <c r="A181" s="7">
+        <f t="shared" si="5"/>
+        <v>174</v>
+      </c>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
-      <c r="D181" s="20"/>
-      <c r="E181" s="19"/>
-      <c r="F181" s="19"/>
-      <c r="G181" s="19"/>
-      <c r="H181" s="19"/>
-      <c r="I181" s="19"/>
+      <c r="D181" s="21"/>
+      <c r="E181" s="20"/>
+      <c r="F181" s="20"/>
+      <c r="G181" s="20"/>
+      <c r="H181" s="20"/>
+      <c r="I181" s="20"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A182" s="7"/>
+      <c r="A182" s="7">
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
-      <c r="D182" s="20"/>
-      <c r="E182" s="19"/>
-      <c r="F182" s="19"/>
-      <c r="G182" s="19"/>
-      <c r="H182" s="19"/>
-      <c r="I182" s="19"/>
+      <c r="D182" s="21"/>
+      <c r="E182" s="20"/>
+      <c r="F182" s="20"/>
+      <c r="G182" s="20"/>
+      <c r="H182" s="20"/>
+      <c r="I182" s="20"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A183" s="7"/>
+      <c r="A183" s="7">
+        <f t="shared" si="5"/>
+        <v>176</v>
+      </c>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
-      <c r="D183" s="20"/>
-      <c r="E183" s="19"/>
-      <c r="F183" s="19"/>
-      <c r="G183" s="19"/>
-      <c r="H183" s="19"/>
-      <c r="I183" s="19"/>
+      <c r="D183" s="21"/>
+      <c r="E183" s="20"/>
+      <c r="F183" s="20"/>
+      <c r="G183" s="20"/>
+      <c r="H183" s="20"/>
+      <c r="I183" s="20"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A184" s="7"/>
+      <c r="A184" s="7">
+        <f t="shared" si="5"/>
+        <v>177</v>
+      </c>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
-      <c r="D184" s="20"/>
-      <c r="E184" s="19"/>
-      <c r="F184" s="19"/>
-      <c r="G184" s="19"/>
-      <c r="H184" s="19"/>
-      <c r="I184" s="19"/>
+      <c r="D184" s="21"/>
+      <c r="E184" s="20"/>
+      <c r="F184" s="20"/>
+      <c r="G184" s="20"/>
+      <c r="H184" s="20"/>
+      <c r="I184" s="20"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A185" s="7"/>
+      <c r="A185" s="7">
+        <f t="shared" si="5"/>
+        <v>178</v>
+      </c>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
-      <c r="D185" s="20"/>
-      <c r="E185" s="19"/>
-      <c r="F185" s="19"/>
-      <c r="G185" s="19"/>
-      <c r="H185" s="19"/>
-      <c r="I185" s="19"/>
+      <c r="D185" s="21"/>
+      <c r="E185" s="20"/>
+      <c r="F185" s="20"/>
+      <c r="G185" s="20"/>
+      <c r="H185" s="20"/>
+      <c r="I185" s="20"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A186" s="7"/>
+      <c r="A186" s="7">
+        <f t="shared" si="5"/>
+        <v>179</v>
+      </c>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
-      <c r="D186" s="20"/>
-      <c r="E186" s="19"/>
-      <c r="F186" s="19"/>
-      <c r="G186" s="19"/>
-      <c r="H186" s="19"/>
-      <c r="I186" s="19"/>
+      <c r="D186" s="21"/>
+      <c r="E186" s="20"/>
+      <c r="F186" s="20"/>
+      <c r="G186" s="20"/>
+      <c r="H186" s="20"/>
+      <c r="I186" s="20"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A187" s="7"/>
+      <c r="A187" s="7">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
-      <c r="D187" s="20"/>
-      <c r="E187" s="19"/>
-      <c r="F187" s="19"/>
-      <c r="G187" s="19"/>
-      <c r="H187" s="19"/>
-      <c r="I187" s="19"/>
+      <c r="D187" s="21"/>
+      <c r="E187" s="20"/>
+      <c r="F187" s="20"/>
+      <c r="G187" s="20"/>
+      <c r="H187" s="20"/>
+      <c r="I187" s="20"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A188" s="7"/>
+      <c r="A188" s="7">
+        <f t="shared" si="5"/>
+        <v>181</v>
+      </c>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
-      <c r="D188" s="20"/>
-      <c r="E188" s="19"/>
-      <c r="F188" s="19"/>
-      <c r="G188" s="19"/>
-      <c r="H188" s="19"/>
-      <c r="I188" s="19"/>
+      <c r="D188" s="21"/>
+      <c r="E188" s="20"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="20"/>
+      <c r="H188" s="20"/>
+      <c r="I188" s="20"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A189" s="7"/>
+      <c r="A189" s="7">
+        <f t="shared" si="5"/>
+        <v>182</v>
+      </c>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
-      <c r="D189" s="20"/>
-      <c r="E189" s="19"/>
-      <c r="F189" s="19"/>
-      <c r="G189" s="19"/>
-      <c r="H189" s="19"/>
-      <c r="I189" s="19"/>
+      <c r="D189" s="21"/>
+      <c r="E189" s="20"/>
+      <c r="F189" s="20"/>
+      <c r="G189" s="20"/>
+      <c r="H189" s="20"/>
+      <c r="I189" s="20"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A190" s="7"/>
+      <c r="A190" s="7">
+        <f t="shared" si="5"/>
+        <v>183</v>
+      </c>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
-      <c r="D190" s="20"/>
-      <c r="E190" s="19"/>
-      <c r="F190" s="19"/>
-      <c r="G190" s="19"/>
-      <c r="H190" s="19"/>
-      <c r="I190" s="19"/>
+      <c r="D190" s="21"/>
+      <c r="E190" s="20"/>
+      <c r="F190" s="20"/>
+      <c r="G190" s="20"/>
+      <c r="H190" s="20"/>
+      <c r="I190" s="20"/>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A191" s="7"/>
+      <c r="A191" s="7">
+        <f t="shared" si="5"/>
+        <v>184</v>
+      </c>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
-      <c r="D191" s="20"/>
-      <c r="E191" s="19"/>
-      <c r="F191" s="19"/>
-      <c r="G191" s="19"/>
-      <c r="H191" s="19"/>
-      <c r="I191" s="19"/>
+      <c r="D191" s="21"/>
+      <c r="E191" s="20"/>
+      <c r="F191" s="20"/>
+      <c r="G191" s="20"/>
+      <c r="H191" s="20"/>
+      <c r="I191" s="20"/>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A192" s="7"/>
+      <c r="A192" s="7">
+        <f t="shared" si="5"/>
+        <v>185</v>
+      </c>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
-      <c r="D192" s="20"/>
-      <c r="E192" s="19"/>
-      <c r="F192" s="19"/>
-      <c r="G192" s="19"/>
-      <c r="H192" s="19"/>
-      <c r="I192" s="19"/>
+      <c r="D192" s="21"/>
+      <c r="E192" s="20"/>
+      <c r="F192" s="20"/>
+      <c r="G192" s="20"/>
+      <c r="H192" s="20"/>
+      <c r="I192" s="20"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A193" s="7"/>
+      <c r="A193" s="7">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
-      <c r="D193" s="19"/>
-      <c r="E193" s="19"/>
-      <c r="F193" s="19"/>
-      <c r="G193" s="19"/>
-      <c r="H193" s="19"/>
-      <c r="I193" s="19"/>
+      <c r="D193" s="20"/>
+      <c r="E193" s="20"/>
+      <c r="F193" s="20"/>
+      <c r="G193" s="20"/>
+      <c r="H193" s="20"/>
+      <c r="I193" s="20"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A194" s="7"/>
+      <c r="A194" s="7">
+        <f t="shared" si="5"/>
+        <v>187</v>
+      </c>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
-      <c r="D194" s="19"/>
-      <c r="E194" s="19"/>
-      <c r="F194" s="19"/>
-      <c r="G194" s="19"/>
-      <c r="H194" s="19"/>
-      <c r="I194" s="19"/>
+      <c r="D194" s="20"/>
+      <c r="E194" s="20"/>
+      <c r="F194" s="20"/>
+      <c r="G194" s="20"/>
+      <c r="H194" s="20"/>
+      <c r="I194" s="20"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A195" s="7"/>
+      <c r="A195" s="7">
+        <f t="shared" si="5"/>
+        <v>188</v>
+      </c>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
-      <c r="D195" s="19"/>
-      <c r="E195" s="19"/>
-      <c r="F195" s="19"/>
-      <c r="G195" s="19"/>
-      <c r="H195" s="19"/>
-      <c r="I195" s="19"/>
+      <c r="D195" s="20"/>
+      <c r="E195" s="20"/>
+      <c r="F195" s="20"/>
+      <c r="G195" s="20"/>
+      <c r="H195" s="20"/>
+      <c r="I195" s="20"/>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A196" s="7"/>
+      <c r="A196" s="7">
+        <f t="shared" si="5"/>
+        <v>189</v>
+      </c>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
-      <c r="D196" s="19"/>
-      <c r="E196" s="19"/>
-      <c r="F196" s="19"/>
-      <c r="G196" s="19"/>
-      <c r="H196" s="19"/>
-      <c r="I196" s="19"/>
+      <c r="D196" s="20"/>
+      <c r="E196" s="20"/>
+      <c r="F196" s="20"/>
+      <c r="G196" s="20"/>
+      <c r="H196" s="20"/>
+      <c r="I196" s="20"/>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A197" s="7"/>
+      <c r="A197" s="7">
+        <f t="shared" si="5"/>
+        <v>190</v>
+      </c>
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
-      <c r="D197" s="20"/>
-      <c r="E197" s="19"/>
-      <c r="F197" s="19"/>
-      <c r="G197" s="19"/>
-      <c r="H197" s="19"/>
-      <c r="I197" s="19"/>
+      <c r="D197" s="21"/>
+      <c r="E197" s="20"/>
+      <c r="F197" s="20"/>
+      <c r="G197" s="20"/>
+      <c r="H197" s="20"/>
+      <c r="I197" s="20"/>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A198" s="7"/>
+      <c r="A198" s="7">
+        <f t="shared" si="5"/>
+        <v>191</v>
+      </c>
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
-      <c r="D198" s="20"/>
-      <c r="E198" s="19"/>
-      <c r="F198" s="19"/>
-      <c r="G198" s="19"/>
-      <c r="H198" s="19"/>
-      <c r="I198" s="19"/>
+      <c r="D198" s="21"/>
+      <c r="E198" s="20"/>
+      <c r="F198" s="20"/>
+      <c r="G198" s="20"/>
+      <c r="H198" s="20"/>
+      <c r="I198" s="20"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A199" s="7"/>
+      <c r="A199" s="7">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
-      <c r="D199" s="20"/>
-      <c r="E199" s="19"/>
-      <c r="F199" s="19"/>
-      <c r="G199" s="19"/>
-      <c r="H199" s="19"/>
-      <c r="I199" s="19"/>
+      <c r="D199" s="21"/>
+      <c r="E199" s="20"/>
+      <c r="F199" s="20"/>
+      <c r="G199" s="20"/>
+      <c r="H199" s="20"/>
+      <c r="I199" s="20"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A200" s="9"/>
+      <c r="A200" s="9">
+        <f t="shared" ref="A200:A231" si="6">ROW(193:200)</f>
+        <v>193</v>
+      </c>
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
-      <c r="D200" s="21"/>
-      <c r="E200" s="19"/>
-      <c r="F200" s="19"/>
-      <c r="G200" s="19"/>
-      <c r="H200" s="19"/>
-      <c r="I200" s="19"/>
+      <c r="D200" s="22"/>
+      <c r="E200" s="20"/>
+      <c r="F200" s="20"/>
+      <c r="G200" s="20"/>
+      <c r="H200" s="20"/>
+      <c r="I200" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:I200">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>OR($C8="Select_Dropdown",$C8="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:I200">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Admin_Portal_Login",$C8="Browser_Quit",$C8="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:F200 H8:I200">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data",$C8="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E200 H8:I200">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>OR($C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D200 H8:I200">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>OR($C8="Portal_Login",$C8="Handle_Browser_window",$C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title",$C8="Open_Portal_URL",$C8="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3692,15 +4285,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Lists!$A$2:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>C8:C200</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Lists!$D$2:$D$14</xm:f>
           </x14:formula1>
           <xm:sqref>E8:E200 G8:G200</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$27</xm:f>
-          </x14:formula1>
-          <xm:sqref>C8:C200</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3710,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3725,14 +4318,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="18"/>
+        <v>42</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="19"/>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3741,7 +4334,7 @@
       </c>
       <c r="B2" s="14"/>
       <c r="D2" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3750,7 +4343,7 @@
       </c>
       <c r="B3" s="14"/>
       <c r="D3" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3759,7 +4352,7 @@
       </c>
       <c r="B4" s="14"/>
       <c r="D4" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3768,7 +4361,7 @@
       </c>
       <c r="B5" s="15"/>
       <c r="D5" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3779,7 +4372,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3788,7 +4381,7 @@
       </c>
       <c r="B7" s="15"/>
       <c r="D7" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3797,7 +4390,7 @@
       </c>
       <c r="B8" s="15"/>
       <c r="D8" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3806,7 +4399,7 @@
       </c>
       <c r="B9" s="15"/>
       <c r="D9" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3815,7 +4408,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="D10" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3824,7 +4417,7 @@
       </c>
       <c r="B11" s="15"/>
       <c r="D11" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3833,7 +4426,7 @@
       </c>
       <c r="B12" s="15"/>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3842,7 +4435,7 @@
       </c>
       <c r="B13" s="15"/>
       <c r="D13" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3851,7 +4444,7 @@
       </c>
       <c r="B14" s="15"/>
       <c r="D14" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3936,6 +4529,22 @@
       </c>
       <c r="B27" s="15" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test cases, updated code to stop using the test suite TS spreadsheet instead to use the location of all the test specs instead
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/QA_Tools/taf/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/GitHub/TAF/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31080" windowHeight="18720" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="31080" windowHeight="18720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Spec" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
-  <si>
-    <t>Project_Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Project_ID</t>
   </si>
   <si>
-    <t>Sprint</t>
-  </si>
-  <si>
     <t>Test_ID</t>
   </si>
   <si>
@@ -139,18 +133,6 @@
   </si>
   <si>
     <t>Custom Function to login to portal</t>
-  </si>
-  <si>
-    <t>SINT_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to sint</t>
-  </si>
-  <si>
-    <t>Admin_Portal_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to Admin portal</t>
   </si>
   <si>
     <t>Notes</t>
@@ -389,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,10 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -447,73 +425,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -679,68 +591,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -913,6 +763,22 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1074,6 +940,56 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1085,113 +1001,61 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>210950</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect b="23077"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8686800" y="215900"/>
-          <a:ext cx="3957450" cy="635000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <tableColumns count="3">
-    <tableColumn id="1" name="Project_Name" dataDxfId="43"/>
-    <tableColumn id="2" name="Project_ID" dataDxfId="42"/>
-    <tableColumn id="3" name="Sprint" dataDxfId="41"/>
+    <tableColumn id="1" name="Test_ID" dataDxfId="32"/>
+    <tableColumn id="2" name="Project_ID" dataDxfId="31"/>
+    <tableColumn id="3" name="Test_Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A7:I200" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="9">
-    <tableColumn id="1" name="Test_Step" dataDxfId="0">
-      <calculatedColumnFormula>ROW(1:8)</calculatedColumnFormula>
+    <tableColumn id="1" name="Test_Step" dataDxfId="24">
+      <calculatedColumnFormula>ROW(1:5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Test_Step_Description" dataDxfId="35"/>
-    <tableColumn id="3" name="Test_Step_Function" dataDxfId="34"/>
-    <tableColumn id="4" name="Test_Step_Value" dataDxfId="33"/>
-    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="32"/>
-    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="31"/>
-    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="30"/>
-    <tableColumn id="8" name="Screenshot" dataDxfId="29"/>
-    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="28"/>
+    <tableColumn id="2" name="Test_Step_Description" dataDxfId="23"/>
+    <tableColumn id="3" name="Test_Step_Function" dataDxfId="22"/>
+    <tableColumn id="4" name="Test_Step_Value" dataDxfId="21"/>
+    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="20"/>
+    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="19"/>
+    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="18"/>
+    <tableColumn id="8" name="Screenshot" dataDxfId="17"/>
+    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:B5" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <tableColumns count="2">
-    <tableColumn id="1" name="Test_ID" dataDxfId="23"/>
-    <tableColumn id="2" name="Test_Description" dataDxfId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:A29"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A1:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="D1:D14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="16"/>
+    <tableColumn id="1" name="Ruby_Locator" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="D1:D14"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Locator" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B29"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Notes" dataDxfId="6"/>
+    <tableColumn id="1" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1460,11 +1324,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I200"/>
+  <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,10 +1346,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1500,100 +1364,128 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="1">
+        <f>ROW(1:5)</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <f>ROW(2:6)</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="A7" s="7">
+        <f>ROW(3:7)</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <f t="shared" ref="A8:A39" si="0">ROW(1:8)</f>
-        <v>1</v>
+      <c r="A8" s="7">
+        <f>ROW(4:8)</f>
+        <v>4</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROW(4:9)</f>
+        <v>4</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROW(4:10)</f>
+        <v>4</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A11:A36" si="0">ROW(4:11)</f>
         <v>4</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -1602,12 +1494,12 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
@@ -1616,12 +1508,12 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -1630,12 +1522,12 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -1644,12 +1536,12 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1658,12 +1550,12 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1672,12 +1564,12 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1686,12 +1578,12 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -1700,12 +1592,12 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1714,12 +1606,12 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1728,12 +1620,12 @@
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1742,12 +1634,12 @@
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -1756,12 +1648,12 @@
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1770,12 +1662,12 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
@@ -1784,12 +1676,12 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -1798,12 +1690,12 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
@@ -1812,12 +1704,12 @@
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
@@ -1826,12 +1718,12 @@
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
@@ -1840,12 +1732,12 @@
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
@@ -1854,12 +1746,12 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
@@ -1868,12 +1760,12 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
@@ -1882,12 +1774,12 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
@@ -1896,12 +1788,12 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
@@ -1910,12 +1802,12 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
@@ -1924,12 +1816,12 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
@@ -1938,68 +1830,68 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A37:A68" si="1">ROW(30:37)</f>
         <v>30</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
-        <f t="shared" ref="A40:A71" si="1">ROW(33:40)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -2008,12 +1900,12 @@
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
@@ -2022,12 +1914,12 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
@@ -2036,12 +1928,12 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -2050,12 +1942,12 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
@@ -2064,12 +1956,12 @@
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
@@ -2078,12 +1970,12 @@
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
@@ -2092,12 +1984,12 @@
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
@@ -2106,12 +1998,12 @@
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
@@ -2120,12 +2012,12 @@
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
@@ -2134,12 +2026,12 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
@@ -2148,12 +2040,12 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
@@ -2162,12 +2054,12 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
@@ -2176,12 +2068,12 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
@@ -2190,12 +2082,12 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
@@ -2204,12 +2096,12 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
@@ -2218,12 +2110,12 @@
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
@@ -2232,12 +2124,12 @@
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
@@ -2246,12 +2138,12 @@
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
@@ -2260,12 +2152,12 @@
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
@@ -2274,12 +2166,12 @@
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
@@ -2288,12 +2180,12 @@
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
@@ -2302,12 +2194,12 @@
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
@@ -2316,12 +2208,12 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
@@ -2330,12 +2222,12 @@
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
@@ -2344,12 +2236,12 @@
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
@@ -2358,12 +2250,12 @@
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-      <c r="H66" s="20"/>
-      <c r="I66" s="20"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
@@ -2372,12 +2264,12 @@
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="20"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
@@ -2386,68 +2278,68 @@
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
-      <c r="H68" s="20"/>
-      <c r="I68" s="20"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A69:A100" si="2">ROW(62:69)</f>
         <v>62</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="20"/>
-      <c r="I69" s="20"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="20"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
-        <f t="shared" ref="A72:A103" si="2">ROW(65:72)</f>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="20"/>
-      <c r="H72" s="20"/>
-      <c r="I72" s="20"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
@@ -2456,12 +2348,12 @@
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="20"/>
-      <c r="H73" s="20"/>
-      <c r="I73" s="20"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -2470,12 +2362,12 @@
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="20"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -2484,12 +2376,12 @@
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20"/>
-      <c r="I75" s="20"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
@@ -2498,12 +2390,12 @@
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="20"/>
-      <c r="H76" s="20"/>
-      <c r="I76" s="20"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -2512,12 +2404,12 @@
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="20"/>
-      <c r="H77" s="20"/>
-      <c r="I77" s="20"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -2526,12 +2418,12 @@
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="20"/>
-      <c r="I78" s="20"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -2540,12 +2432,12 @@
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="20"/>
-      <c r="I79" s="20"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -2554,12 +2446,12 @@
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
-      <c r="I80" s="20"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
@@ -2568,12 +2460,12 @@
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="20"/>
-      <c r="H81" s="20"/>
-      <c r="I81" s="20"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
@@ -2582,12 +2474,12 @@
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-      <c r="I82" s="20"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
@@ -2596,12 +2488,12 @@
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="20"/>
-      <c r="I83" s="20"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
@@ -2610,12 +2502,12 @@
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
-      <c r="I84" s="20"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
@@ -2624,12 +2516,12 @@
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="20"/>
-      <c r="I85" s="20"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
@@ -2638,12 +2530,12 @@
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="20"/>
-      <c r="H86" s="20"/>
-      <c r="I86" s="20"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
@@ -2652,12 +2544,12 @@
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="20"/>
-      <c r="H87" s="20"/>
-      <c r="I87" s="20"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
@@ -2666,12 +2558,12 @@
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="20"/>
-      <c r="I88" s="20"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
@@ -2680,12 +2572,12 @@
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="20"/>
-      <c r="I89" s="20"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
@@ -2694,12 +2586,12 @@
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="20"/>
-      <c r="I90" s="20"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
@@ -2708,12 +2600,12 @@
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
-      <c r="G91" s="20"/>
-      <c r="H91" s="20"/>
-      <c r="I91" s="20"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
@@ -2722,12 +2614,12 @@
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="20"/>
-      <c r="I92" s="20"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
@@ -2736,12 +2628,12 @@
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20"/>
-      <c r="H93" s="20"/>
-      <c r="I93" s="20"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
@@ -2750,12 +2642,12 @@
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
@@ -2764,12 +2656,12 @@
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="20"/>
-      <c r="I95" s="20"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
@@ -2778,12 +2670,12 @@
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="20"/>
-      <c r="H96" s="20"/>
-      <c r="I96" s="20"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
@@ -2792,12 +2684,12 @@
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="20"/>
-      <c r="H97" s="20"/>
-      <c r="I97" s="20"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -2806,12 +2698,12 @@
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="20"/>
-      <c r="H98" s="20"/>
-      <c r="I98" s="20"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
@@ -2820,12 +2712,12 @@
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="20"/>
-      <c r="G99" s="20"/>
-      <c r="H99" s="20"/>
-      <c r="I99" s="20"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
@@ -2834,68 +2726,68 @@
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="20"/>
-      <c r="H100" s="20"/>
-      <c r="I100" s="20"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A101:A132" si="3">ROW(94:101)</f>
         <v>94</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="20"/>
-      <c r="H101" s="20"/>
-      <c r="I101" s="20"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="20"/>
-      <c r="I102" s="20"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="20"/>
-      <c r="H103" s="20"/>
-      <c r="I103" s="20"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
-        <f t="shared" ref="A104:A135" si="3">ROW(97:104)</f>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="20"/>
-      <c r="I104" s="20"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -2904,12 +2796,12 @@
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="20"/>
-      <c r="I105" s="20"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
@@ -2918,12 +2810,12 @@
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="20"/>
-      <c r="I106" s="20"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -2932,12 +2824,12 @@
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="20"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="18"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -2946,12 +2838,12 @@
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="20"/>
-      <c r="I108" s="20"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="18"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -2960,12 +2852,12 @@
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="20"/>
-      <c r="I109" s="20"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -2974,12 +2866,12 @@
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
@@ -2988,12 +2880,12 @@
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
-      <c r="D111" s="20"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="18"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
@@ -3002,12 +2894,12 @@
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
-      <c r="D112" s="20"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="20"/>
-      <c r="I112" s="20"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="18"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
@@ -3016,12 +2908,12 @@
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="18"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
@@ -3030,12 +2922,12 @@
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
-      <c r="D114" s="20"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="20"/>
-      <c r="H114" s="20"/>
-      <c r="I114" s="20"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
@@ -3044,12 +2936,12 @@
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
-      <c r="D115" s="20"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="20"/>
-      <c r="H115" s="20"/>
-      <c r="I115" s="20"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="18"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
@@ -3058,12 +2950,12 @@
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
-      <c r="D116" s="20"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="20"/>
-      <c r="G116" s="20"/>
-      <c r="H116" s="20"/>
-      <c r="I116" s="20"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
@@ -3072,12 +2964,12 @@
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
-      <c r="D117" s="20"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="20"/>
-      <c r="G117" s="20"/>
-      <c r="H117" s="20"/>
-      <c r="I117" s="20"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+      <c r="I117" s="18"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
@@ -3086,12 +2978,12 @@
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="20"/>
-      <c r="H118" s="20"/>
-      <c r="I118" s="20"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
+      <c r="G118" s="18"/>
+      <c r="H118" s="18"/>
+      <c r="I118" s="18"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
@@ -3100,12 +2992,12 @@
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
-      <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20"/>
-      <c r="H119" s="20"/>
-      <c r="I119" s="20"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+      <c r="G119" s="18"/>
+      <c r="H119" s="18"/>
+      <c r="I119" s="18"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
@@ -3114,12 +3006,12 @@
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
-      <c r="D120" s="20"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="20"/>
-      <c r="H120" s="20"/>
-      <c r="I120" s="20"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
+      <c r="H120" s="18"/>
+      <c r="I120" s="18"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
@@ -3128,12 +3020,12 @@
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
-      <c r="D121" s="20"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="20"/>
-      <c r="H121" s="20"/>
-      <c r="I121" s="20"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="18"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+      <c r="H121" s="18"/>
+      <c r="I121" s="18"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
@@ -3142,12 +3034,12 @@
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="20"/>
-      <c r="H122" s="20"/>
-      <c r="I122" s="20"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+      <c r="H122" s="18"/>
+      <c r="I122" s="18"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
@@ -3156,12 +3048,12 @@
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="20"/>
-      <c r="H123" s="20"/>
-      <c r="I123" s="20"/>
+      <c r="D123" s="18"/>
+      <c r="E123" s="18"/>
+      <c r="F123" s="18"/>
+      <c r="G123" s="18"/>
+      <c r="H123" s="18"/>
+      <c r="I123" s="18"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
@@ -3170,12 +3062,12 @@
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
-      <c r="D124" s="20"/>
-      <c r="E124" s="20"/>
-      <c r="F124" s="20"/>
-      <c r="G124" s="20"/>
-      <c r="H124" s="20"/>
-      <c r="I124" s="20"/>
+      <c r="D124" s="18"/>
+      <c r="E124" s="18"/>
+      <c r="F124" s="18"/>
+      <c r="G124" s="18"/>
+      <c r="H124" s="18"/>
+      <c r="I124" s="18"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
@@ -3184,12 +3076,12 @@
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="20"/>
-      <c r="H125" s="20"/>
-      <c r="I125" s="20"/>
+      <c r="D125" s="18"/>
+      <c r="E125" s="18"/>
+      <c r="F125" s="18"/>
+      <c r="G125" s="18"/>
+      <c r="H125" s="18"/>
+      <c r="I125" s="18"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
@@ -3198,12 +3090,12 @@
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
-      <c r="D126" s="20"/>
-      <c r="E126" s="20"/>
-      <c r="F126" s="20"/>
-      <c r="G126" s="20"/>
-      <c r="H126" s="20"/>
-      <c r="I126" s="20"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
+      <c r="I126" s="18"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
@@ -3212,12 +3104,12 @@
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
-      <c r="D127" s="20"/>
-      <c r="E127" s="20"/>
-      <c r="F127" s="20"/>
-      <c r="G127" s="20"/>
-      <c r="H127" s="20"/>
-      <c r="I127" s="20"/>
+      <c r="D127" s="18"/>
+      <c r="E127" s="18"/>
+      <c r="F127" s="18"/>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18"/>
+      <c r="I127" s="18"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
@@ -3226,12 +3118,12 @@
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
-      <c r="D128" s="20"/>
-      <c r="E128" s="20"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="20"/>
-      <c r="H128" s="20"/>
-      <c r="I128" s="20"/>
+      <c r="D128" s="18"/>
+      <c r="E128" s="18"/>
+      <c r="F128" s="18"/>
+      <c r="G128" s="18"/>
+      <c r="H128" s="18"/>
+      <c r="I128" s="18"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
@@ -3240,12 +3132,12 @@
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
-      <c r="D129" s="20"/>
-      <c r="E129" s="20"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="20"/>
-      <c r="H129" s="20"/>
-      <c r="I129" s="20"/>
+      <c r="D129" s="18"/>
+      <c r="E129" s="18"/>
+      <c r="F129" s="18"/>
+      <c r="G129" s="18"/>
+      <c r="H129" s="18"/>
+      <c r="I129" s="18"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -3254,12 +3146,12 @@
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="20"/>
-      <c r="E130" s="20"/>
-      <c r="F130" s="20"/>
-      <c r="G130" s="20"/>
-      <c r="H130" s="20"/>
-      <c r="I130" s="20"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="18"/>
+      <c r="H130" s="18"/>
+      <c r="I130" s="18"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -3268,12 +3160,12 @@
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
-      <c r="D131" s="20"/>
-      <c r="E131" s="20"/>
-      <c r="F131" s="20"/>
-      <c r="G131" s="20"/>
-      <c r="H131" s="20"/>
-      <c r="I131" s="20"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="18"/>
+      <c r="F131" s="18"/>
+      <c r="G131" s="18"/>
+      <c r="H131" s="18"/>
+      <c r="I131" s="18"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="7">
@@ -3282,68 +3174,68 @@
       </c>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
-      <c r="D132" s="20"/>
-      <c r="E132" s="20"/>
-      <c r="F132" s="20"/>
-      <c r="G132" s="20"/>
-      <c r="H132" s="20"/>
-      <c r="I132" s="20"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="18"/>
+      <c r="F132" s="18"/>
+      <c r="G132" s="18"/>
+      <c r="H132" s="18"/>
+      <c r="I132" s="18"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A133:A164" si="4">ROW(126:133)</f>
         <v>126</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
-      <c r="D133" s="20"/>
-      <c r="E133" s="20"/>
-      <c r="F133" s="20"/>
-      <c r="G133" s="20"/>
-      <c r="H133" s="20"/>
-      <c r="I133" s="20"/>
+      <c r="D133" s="19"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="18"/>
+      <c r="G133" s="18"/>
+      <c r="H133" s="18"/>
+      <c r="I133" s="18"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
-      <c r="D134" s="21"/>
-      <c r="E134" s="20"/>
-      <c r="F134" s="20"/>
-      <c r="G134" s="20"/>
-      <c r="H134" s="20"/>
-      <c r="I134" s="20"/>
+      <c r="D134" s="19"/>
+      <c r="E134" s="18"/>
+      <c r="F134" s="18"/>
+      <c r="G134" s="18"/>
+      <c r="H134" s="18"/>
+      <c r="I134" s="18"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
-      <c r="D135" s="21"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="20"/>
-      <c r="G135" s="20"/>
-      <c r="H135" s="20"/>
-      <c r="I135" s="20"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="18"/>
+      <c r="F135" s="18"/>
+      <c r="G135" s="18"/>
+      <c r="H135" s="18"/>
+      <c r="I135" s="18"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
-        <f t="shared" ref="A136:A167" si="4">ROW(129:136)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
-      <c r="D136" s="21"/>
-      <c r="E136" s="20"/>
-      <c r="F136" s="20"/>
-      <c r="G136" s="20"/>
-      <c r="H136" s="20"/>
-      <c r="I136" s="20"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="18"/>
+      <c r="F136" s="18"/>
+      <c r="G136" s="18"/>
+      <c r="H136" s="18"/>
+      <c r="I136" s="18"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
@@ -3352,12 +3244,12 @@
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
-      <c r="D137" s="21"/>
-      <c r="E137" s="20"/>
-      <c r="F137" s="20"/>
-      <c r="G137" s="20"/>
-      <c r="H137" s="20"/>
-      <c r="I137" s="20"/>
+      <c r="D137" s="19"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="18"/>
+      <c r="H137" s="18"/>
+      <c r="I137" s="18"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
@@ -3366,12 +3258,12 @@
       </c>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
-      <c r="D138" s="21"/>
-      <c r="E138" s="20"/>
-      <c r="F138" s="20"/>
-      <c r="G138" s="20"/>
-      <c r="H138" s="20"/>
-      <c r="I138" s="20"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="18"/>
+      <c r="G138" s="18"/>
+      <c r="H138" s="18"/>
+      <c r="I138" s="18"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
@@ -3380,12 +3272,12 @@
       </c>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
-      <c r="D139" s="21"/>
-      <c r="E139" s="20"/>
-      <c r="F139" s="20"/>
-      <c r="G139" s="20"/>
-      <c r="H139" s="20"/>
-      <c r="I139" s="20"/>
+      <c r="D139" s="19"/>
+      <c r="E139" s="18"/>
+      <c r="F139" s="18"/>
+      <c r="G139" s="18"/>
+      <c r="H139" s="18"/>
+      <c r="I139" s="18"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
@@ -3394,12 +3286,12 @@
       </c>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="21"/>
-      <c r="E140" s="20"/>
-      <c r="F140" s="20"/>
-      <c r="G140" s="20"/>
-      <c r="H140" s="20"/>
-      <c r="I140" s="20"/>
+      <c r="D140" s="19"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="18"/>
+      <c r="G140" s="18"/>
+      <c r="H140" s="18"/>
+      <c r="I140" s="18"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
@@ -3408,12 +3300,12 @@
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
-      <c r="D141" s="21"/>
-      <c r="E141" s="20"/>
-      <c r="F141" s="20"/>
-      <c r="G141" s="20"/>
-      <c r="H141" s="20"/>
-      <c r="I141" s="20"/>
+      <c r="D141" s="19"/>
+      <c r="E141" s="18"/>
+      <c r="F141" s="18"/>
+      <c r="G141" s="18"/>
+      <c r="H141" s="18"/>
+      <c r="I141" s="18"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
@@ -3422,12 +3314,12 @@
       </c>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
-      <c r="D142" s="21"/>
-      <c r="E142" s="20"/>
-      <c r="F142" s="20"/>
-      <c r="G142" s="20"/>
-      <c r="H142" s="20"/>
-      <c r="I142" s="20"/>
+      <c r="D142" s="19"/>
+      <c r="E142" s="18"/>
+      <c r="F142" s="18"/>
+      <c r="G142" s="18"/>
+      <c r="H142" s="18"/>
+      <c r="I142" s="18"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
@@ -3436,12 +3328,12 @@
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
-      <c r="D143" s="21"/>
-      <c r="E143" s="20"/>
-      <c r="F143" s="20"/>
-      <c r="G143" s="20"/>
-      <c r="H143" s="20"/>
-      <c r="I143" s="20"/>
+      <c r="D143" s="19"/>
+      <c r="E143" s="18"/>
+      <c r="F143" s="18"/>
+      <c r="G143" s="18"/>
+      <c r="H143" s="18"/>
+      <c r="I143" s="18"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
@@ -3450,12 +3342,12 @@
       </c>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
-      <c r="D144" s="21"/>
-      <c r="E144" s="20"/>
-      <c r="F144" s="20"/>
-      <c r="G144" s="20"/>
-      <c r="H144" s="20"/>
-      <c r="I144" s="20"/>
+      <c r="D144" s="19"/>
+      <c r="E144" s="18"/>
+      <c r="F144" s="18"/>
+      <c r="G144" s="18"/>
+      <c r="H144" s="18"/>
+      <c r="I144" s="18"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
@@ -3464,12 +3356,12 @@
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
-      <c r="D145" s="21"/>
-      <c r="E145" s="20"/>
-      <c r="F145" s="20"/>
-      <c r="G145" s="20"/>
-      <c r="H145" s="20"/>
-      <c r="I145" s="20"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="18"/>
+      <c r="F145" s="18"/>
+      <c r="G145" s="18"/>
+      <c r="H145" s="18"/>
+      <c r="I145" s="18"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
@@ -3478,12 +3370,12 @@
       </c>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
-      <c r="D146" s="21"/>
-      <c r="E146" s="20"/>
-      <c r="F146" s="20"/>
-      <c r="G146" s="20"/>
-      <c r="H146" s="20"/>
-      <c r="I146" s="20"/>
+      <c r="D146" s="19"/>
+      <c r="E146" s="18"/>
+      <c r="F146" s="18"/>
+      <c r="G146" s="18"/>
+      <c r="H146" s="18"/>
+      <c r="I146" s="18"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
@@ -3492,12 +3384,12 @@
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
-      <c r="D147" s="21"/>
-      <c r="E147" s="20"/>
-      <c r="F147" s="20"/>
-      <c r="G147" s="20"/>
-      <c r="H147" s="20"/>
-      <c r="I147" s="20"/>
+      <c r="D147" s="19"/>
+      <c r="E147" s="18"/>
+      <c r="F147" s="18"/>
+      <c r="G147" s="18"/>
+      <c r="H147" s="18"/>
+      <c r="I147" s="18"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
@@ -3506,12 +3398,12 @@
       </c>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
-      <c r="D148" s="21"/>
-      <c r="E148" s="20"/>
-      <c r="F148" s="20"/>
-      <c r="G148" s="20"/>
-      <c r="H148" s="20"/>
-      <c r="I148" s="20"/>
+      <c r="D148" s="19"/>
+      <c r="E148" s="18"/>
+      <c r="F148" s="18"/>
+      <c r="G148" s="18"/>
+      <c r="H148" s="18"/>
+      <c r="I148" s="18"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
@@ -3520,12 +3412,12 @@
       </c>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
-      <c r="D149" s="21"/>
-      <c r="E149" s="20"/>
-      <c r="F149" s="20"/>
-      <c r="G149" s="20"/>
-      <c r="H149" s="20"/>
-      <c r="I149" s="20"/>
+      <c r="D149" s="19"/>
+      <c r="E149" s="18"/>
+      <c r="F149" s="18"/>
+      <c r="G149" s="18"/>
+      <c r="H149" s="18"/>
+      <c r="I149" s="18"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
@@ -3534,12 +3426,12 @@
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
-      <c r="D150" s="21"/>
-      <c r="E150" s="20"/>
-      <c r="F150" s="20"/>
-      <c r="G150" s="20"/>
-      <c r="H150" s="20"/>
-      <c r="I150" s="20"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="18"/>
+      <c r="F150" s="18"/>
+      <c r="G150" s="18"/>
+      <c r="H150" s="18"/>
+      <c r="I150" s="18"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
@@ -3548,12 +3440,12 @@
       </c>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
-      <c r="D151" s="21"/>
-      <c r="E151" s="20"/>
-      <c r="F151" s="20"/>
-      <c r="G151" s="20"/>
-      <c r="H151" s="20"/>
-      <c r="I151" s="20"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="18"/>
+      <c r="F151" s="18"/>
+      <c r="G151" s="18"/>
+      <c r="H151" s="18"/>
+      <c r="I151" s="18"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
@@ -3562,12 +3454,12 @@
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
-      <c r="D152" s="21"/>
-      <c r="E152" s="20"/>
-      <c r="F152" s="20"/>
-      <c r="G152" s="20"/>
-      <c r="H152" s="20"/>
-      <c r="I152" s="20"/>
+      <c r="D152" s="18"/>
+      <c r="E152" s="18"/>
+      <c r="F152" s="18"/>
+      <c r="G152" s="18"/>
+      <c r="H152" s="18"/>
+      <c r="I152" s="18"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
@@ -3576,12 +3468,12 @@
       </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
-      <c r="D153" s="20"/>
-      <c r="E153" s="20"/>
-      <c r="F153" s="20"/>
-      <c r="G153" s="20"/>
-      <c r="H153" s="20"/>
-      <c r="I153" s="20"/>
+      <c r="D153" s="18"/>
+      <c r="E153" s="18"/>
+      <c r="F153" s="18"/>
+      <c r="G153" s="18"/>
+      <c r="H153" s="18"/>
+      <c r="I153" s="18"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
@@ -3590,12 +3482,12 @@
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
-      <c r="D154" s="20"/>
-      <c r="E154" s="20"/>
-      <c r="F154" s="20"/>
-      <c r="G154" s="20"/>
-      <c r="H154" s="20"/>
-      <c r="I154" s="20"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
+      <c r="I154" s="18"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
@@ -3604,12 +3496,12 @@
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
-      <c r="D155" s="20"/>
-      <c r="E155" s="20"/>
-      <c r="F155" s="20"/>
-      <c r="G155" s="20"/>
-      <c r="H155" s="20"/>
-      <c r="I155" s="20"/>
+      <c r="D155" s="18"/>
+      <c r="E155" s="18"/>
+      <c r="F155" s="18"/>
+      <c r="G155" s="18"/>
+      <c r="H155" s="18"/>
+      <c r="I155" s="18"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
@@ -3618,12 +3510,12 @@
       </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
-      <c r="D156" s="20"/>
-      <c r="E156" s="20"/>
-      <c r="F156" s="20"/>
-      <c r="G156" s="20"/>
-      <c r="H156" s="20"/>
-      <c r="I156" s="20"/>
+      <c r="D156" s="18"/>
+      <c r="E156" s="18"/>
+      <c r="F156" s="18"/>
+      <c r="G156" s="18"/>
+      <c r="H156" s="18"/>
+      <c r="I156" s="18"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
@@ -3632,12 +3524,12 @@
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
-      <c r="D157" s="20"/>
-      <c r="E157" s="20"/>
-      <c r="F157" s="20"/>
-      <c r="G157" s="20"/>
-      <c r="H157" s="20"/>
-      <c r="I157" s="20"/>
+      <c r="D157" s="18"/>
+      <c r="E157" s="18"/>
+      <c r="F157" s="18"/>
+      <c r="G157" s="18"/>
+      <c r="H157" s="18"/>
+      <c r="I157" s="18"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
@@ -3646,12 +3538,12 @@
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
-      <c r="D158" s="20"/>
-      <c r="E158" s="20"/>
-      <c r="F158" s="20"/>
-      <c r="G158" s="20"/>
-      <c r="H158" s="20"/>
-      <c r="I158" s="20"/>
+      <c r="D158" s="18"/>
+      <c r="E158" s="18"/>
+      <c r="F158" s="18"/>
+      <c r="G158" s="18"/>
+      <c r="H158" s="18"/>
+      <c r="I158" s="18"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
@@ -3660,12 +3552,12 @@
       </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
-      <c r="D159" s="20"/>
-      <c r="E159" s="20"/>
-      <c r="F159" s="20"/>
-      <c r="G159" s="20"/>
-      <c r="H159" s="20"/>
-      <c r="I159" s="20"/>
+      <c r="D159" s="18"/>
+      <c r="E159" s="18"/>
+      <c r="F159" s="18"/>
+      <c r="G159" s="18"/>
+      <c r="H159" s="18"/>
+      <c r="I159" s="18"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
@@ -3674,12 +3566,12 @@
       </c>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
-      <c r="D160" s="20"/>
-      <c r="E160" s="20"/>
-      <c r="F160" s="20"/>
-      <c r="G160" s="20"/>
-      <c r="H160" s="20"/>
-      <c r="I160" s="20"/>
+      <c r="D160" s="18"/>
+      <c r="E160" s="18"/>
+      <c r="F160" s="18"/>
+      <c r="G160" s="18"/>
+      <c r="H160" s="18"/>
+      <c r="I160" s="18"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
@@ -3688,12 +3580,12 @@
       </c>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
-      <c r="D161" s="20"/>
-      <c r="E161" s="20"/>
-      <c r="F161" s="20"/>
-      <c r="G161" s="20"/>
-      <c r="H161" s="20"/>
-      <c r="I161" s="20"/>
+      <c r="D161" s="18"/>
+      <c r="E161" s="18"/>
+      <c r="F161" s="18"/>
+      <c r="G161" s="18"/>
+      <c r="H161" s="18"/>
+      <c r="I161" s="18"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
@@ -3702,12 +3594,12 @@
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
-      <c r="D162" s="20"/>
-      <c r="E162" s="20"/>
-      <c r="F162" s="20"/>
-      <c r="G162" s="20"/>
-      <c r="H162" s="20"/>
-      <c r="I162" s="20"/>
+      <c r="D162" s="18"/>
+      <c r="E162" s="18"/>
+      <c r="F162" s="18"/>
+      <c r="G162" s="18"/>
+      <c r="H162" s="18"/>
+      <c r="I162" s="18"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
@@ -3716,12 +3608,12 @@
       </c>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
-      <c r="D163" s="20"/>
-      <c r="E163" s="20"/>
-      <c r="F163" s="20"/>
-      <c r="G163" s="20"/>
-      <c r="H163" s="20"/>
-      <c r="I163" s="20"/>
+      <c r="D163" s="18"/>
+      <c r="E163" s="18"/>
+      <c r="F163" s="18"/>
+      <c r="G163" s="18"/>
+      <c r="H163" s="18"/>
+      <c r="I163" s="18"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
@@ -3730,68 +3622,68 @@
       </c>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
-      <c r="D164" s="20"/>
-      <c r="E164" s="20"/>
-      <c r="F164" s="20"/>
-      <c r="G164" s="20"/>
-      <c r="H164" s="20"/>
-      <c r="I164" s="20"/>
+      <c r="D164" s="18"/>
+      <c r="E164" s="18"/>
+      <c r="F164" s="18"/>
+      <c r="G164" s="18"/>
+      <c r="H164" s="18"/>
+      <c r="I164" s="18"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A165:A196" si="5">ROW(158:165)</f>
         <v>158</v>
       </c>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
-      <c r="D165" s="20"/>
-      <c r="E165" s="20"/>
-      <c r="F165" s="20"/>
-      <c r="G165" s="20"/>
-      <c r="H165" s="20"/>
-      <c r="I165" s="20"/>
+      <c r="D165" s="18"/>
+      <c r="E165" s="18"/>
+      <c r="F165" s="18"/>
+      <c r="G165" s="18"/>
+      <c r="H165" s="18"/>
+      <c r="I165" s="18"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
-      <c r="D166" s="20"/>
-      <c r="E166" s="20"/>
-      <c r="F166" s="20"/>
-      <c r="G166" s="20"/>
-      <c r="H166" s="20"/>
-      <c r="I166" s="20"/>
+      <c r="D166" s="18"/>
+      <c r="E166" s="18"/>
+      <c r="F166" s="18"/>
+      <c r="G166" s="18"/>
+      <c r="H166" s="18"/>
+      <c r="I166" s="18"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
-      <c r="D167" s="20"/>
-      <c r="E167" s="20"/>
-      <c r="F167" s="20"/>
-      <c r="G167" s="20"/>
-      <c r="H167" s="20"/>
-      <c r="I167" s="20"/>
+      <c r="D167" s="18"/>
+      <c r="E167" s="18"/>
+      <c r="F167" s="18"/>
+      <c r="G167" s="18"/>
+      <c r="H167" s="18"/>
+      <c r="I167" s="18"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
-        <f t="shared" ref="A168:A199" si="5">ROW(161:168)</f>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
-      <c r="D168" s="20"/>
-      <c r="E168" s="20"/>
-      <c r="F168" s="20"/>
-      <c r="G168" s="20"/>
-      <c r="H168" s="20"/>
-      <c r="I168" s="20"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
+      <c r="G168" s="18"/>
+      <c r="H168" s="18"/>
+      <c r="I168" s="18"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
@@ -3800,12 +3692,12 @@
       </c>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
-      <c r="D169" s="20"/>
-      <c r="E169" s="20"/>
-      <c r="F169" s="20"/>
-      <c r="G169" s="20"/>
-      <c r="H169" s="20"/>
-      <c r="I169" s="20"/>
+      <c r="D169" s="18"/>
+      <c r="E169" s="18"/>
+      <c r="F169" s="18"/>
+      <c r="G169" s="18"/>
+      <c r="H169" s="18"/>
+      <c r="I169" s="18"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
@@ -3814,12 +3706,12 @@
       </c>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
-      <c r="D170" s="20"/>
-      <c r="E170" s="20"/>
-      <c r="F170" s="20"/>
-      <c r="G170" s="20"/>
-      <c r="H170" s="20"/>
-      <c r="I170" s="20"/>
+      <c r="D170" s="18"/>
+      <c r="E170" s="18"/>
+      <c r="F170" s="18"/>
+      <c r="G170" s="18"/>
+      <c r="H170" s="18"/>
+      <c r="I170" s="18"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
@@ -3828,12 +3720,12 @@
       </c>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
-      <c r="D171" s="20"/>
-      <c r="E171" s="20"/>
-      <c r="F171" s="20"/>
-      <c r="G171" s="20"/>
-      <c r="H171" s="20"/>
-      <c r="I171" s="20"/>
+      <c r="D171" s="18"/>
+      <c r="E171" s="18"/>
+      <c r="F171" s="18"/>
+      <c r="G171" s="18"/>
+      <c r="H171" s="18"/>
+      <c r="I171" s="18"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
@@ -3842,12 +3734,12 @@
       </c>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
-      <c r="D172" s="20"/>
-      <c r="E172" s="20"/>
-      <c r="F172" s="20"/>
-      <c r="G172" s="20"/>
-      <c r="H172" s="20"/>
-      <c r="I172" s="20"/>
+      <c r="D172" s="19"/>
+      <c r="E172" s="18"/>
+      <c r="F172" s="18"/>
+      <c r="G172" s="18"/>
+      <c r="H172" s="18"/>
+      <c r="I172" s="18"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
@@ -3856,12 +3748,12 @@
       </c>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
-      <c r="D173" s="20"/>
-      <c r="E173" s="20"/>
-      <c r="F173" s="20"/>
-      <c r="G173" s="20"/>
-      <c r="H173" s="20"/>
-      <c r="I173" s="20"/>
+      <c r="D173" s="19"/>
+      <c r="E173" s="18"/>
+      <c r="F173" s="18"/>
+      <c r="G173" s="18"/>
+      <c r="H173" s="18"/>
+      <c r="I173" s="18"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
@@ -3870,12 +3762,12 @@
       </c>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
-      <c r="D174" s="20"/>
-      <c r="E174" s="20"/>
-      <c r="F174" s="20"/>
-      <c r="G174" s="20"/>
-      <c r="H174" s="20"/>
-      <c r="I174" s="20"/>
+      <c r="D174" s="19"/>
+      <c r="E174" s="18"/>
+      <c r="F174" s="18"/>
+      <c r="G174" s="18"/>
+      <c r="H174" s="18"/>
+      <c r="I174" s="18"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
@@ -3884,12 +3776,12 @@
       </c>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
-      <c r="D175" s="21"/>
-      <c r="E175" s="20"/>
-      <c r="F175" s="20"/>
-      <c r="G175" s="20"/>
-      <c r="H175" s="20"/>
-      <c r="I175" s="20"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="18"/>
+      <c r="F175" s="18"/>
+      <c r="G175" s="18"/>
+      <c r="H175" s="18"/>
+      <c r="I175" s="18"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
@@ -3898,12 +3790,12 @@
       </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
-      <c r="D176" s="21"/>
-      <c r="E176" s="20"/>
-      <c r="F176" s="20"/>
-      <c r="G176" s="20"/>
-      <c r="H176" s="20"/>
-      <c r="I176" s="20"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="18"/>
+      <c r="F176" s="18"/>
+      <c r="G176" s="18"/>
+      <c r="H176" s="18"/>
+      <c r="I176" s="18"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
@@ -3912,12 +3804,12 @@
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="21"/>
-      <c r="E177" s="20"/>
-      <c r="F177" s="20"/>
-      <c r="G177" s="20"/>
-      <c r="H177" s="20"/>
-      <c r="I177" s="20"/>
+      <c r="D177" s="19"/>
+      <c r="E177" s="18"/>
+      <c r="F177" s="18"/>
+      <c r="G177" s="18"/>
+      <c r="H177" s="18"/>
+      <c r="I177" s="18"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
@@ -3926,12 +3818,12 @@
       </c>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="21"/>
-      <c r="E178" s="20"/>
-      <c r="F178" s="20"/>
-      <c r="G178" s="20"/>
-      <c r="H178" s="20"/>
-      <c r="I178" s="20"/>
+      <c r="D178" s="19"/>
+      <c r="E178" s="18"/>
+      <c r="F178" s="18"/>
+      <c r="G178" s="18"/>
+      <c r="H178" s="18"/>
+      <c r="I178" s="18"/>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
@@ -3940,12 +3832,12 @@
       </c>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
-      <c r="D179" s="21"/>
-      <c r="E179" s="20"/>
-      <c r="F179" s="20"/>
-      <c r="G179" s="20"/>
-      <c r="H179" s="20"/>
-      <c r="I179" s="20"/>
+      <c r="D179" s="19"/>
+      <c r="E179" s="18"/>
+      <c r="F179" s="18"/>
+      <c r="G179" s="18"/>
+      <c r="H179" s="18"/>
+      <c r="I179" s="18"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
@@ -3954,12 +3846,12 @@
       </c>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
-      <c r="D180" s="21"/>
-      <c r="E180" s="20"/>
-      <c r="F180" s="20"/>
-      <c r="G180" s="20"/>
-      <c r="H180" s="20"/>
-      <c r="I180" s="20"/>
+      <c r="D180" s="19"/>
+      <c r="E180" s="18"/>
+      <c r="F180" s="18"/>
+      <c r="G180" s="18"/>
+      <c r="H180" s="18"/>
+      <c r="I180" s="18"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
@@ -3968,12 +3860,12 @@
       </c>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
-      <c r="D181" s="21"/>
-      <c r="E181" s="20"/>
-      <c r="F181" s="20"/>
-      <c r="G181" s="20"/>
-      <c r="H181" s="20"/>
-      <c r="I181" s="20"/>
+      <c r="D181" s="19"/>
+      <c r="E181" s="18"/>
+      <c r="F181" s="18"/>
+      <c r="G181" s="18"/>
+      <c r="H181" s="18"/>
+      <c r="I181" s="18"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
@@ -3982,12 +3874,12 @@
       </c>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
-      <c r="D182" s="21"/>
-      <c r="E182" s="20"/>
-      <c r="F182" s="20"/>
-      <c r="G182" s="20"/>
-      <c r="H182" s="20"/>
-      <c r="I182" s="20"/>
+      <c r="D182" s="19"/>
+      <c r="E182" s="18"/>
+      <c r="F182" s="18"/>
+      <c r="G182" s="18"/>
+      <c r="H182" s="18"/>
+      <c r="I182" s="18"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
@@ -3996,12 +3888,12 @@
       </c>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
-      <c r="D183" s="21"/>
-      <c r="E183" s="20"/>
-      <c r="F183" s="20"/>
-      <c r="G183" s="20"/>
-      <c r="H183" s="20"/>
-      <c r="I183" s="20"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="18"/>
+      <c r="F183" s="18"/>
+      <c r="G183" s="18"/>
+      <c r="H183" s="18"/>
+      <c r="I183" s="18"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
@@ -4010,12 +3902,12 @@
       </c>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
-      <c r="D184" s="21"/>
-      <c r="E184" s="20"/>
-      <c r="F184" s="20"/>
-      <c r="G184" s="20"/>
-      <c r="H184" s="20"/>
-      <c r="I184" s="20"/>
+      <c r="D184" s="19"/>
+      <c r="E184" s="18"/>
+      <c r="F184" s="18"/>
+      <c r="G184" s="18"/>
+      <c r="H184" s="18"/>
+      <c r="I184" s="18"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
@@ -4024,12 +3916,12 @@
       </c>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
-      <c r="D185" s="21"/>
-      <c r="E185" s="20"/>
-      <c r="F185" s="20"/>
-      <c r="G185" s="20"/>
-      <c r="H185" s="20"/>
-      <c r="I185" s="20"/>
+      <c r="D185" s="19"/>
+      <c r="E185" s="18"/>
+      <c r="F185" s="18"/>
+      <c r="G185" s="18"/>
+      <c r="H185" s="18"/>
+      <c r="I185" s="18"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
@@ -4038,12 +3930,12 @@
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
-      <c r="D186" s="21"/>
-      <c r="E186" s="20"/>
-      <c r="F186" s="20"/>
-      <c r="G186" s="20"/>
-      <c r="H186" s="20"/>
-      <c r="I186" s="20"/>
+      <c r="D186" s="19"/>
+      <c r="E186" s="18"/>
+      <c r="F186" s="18"/>
+      <c r="G186" s="18"/>
+      <c r="H186" s="18"/>
+      <c r="I186" s="18"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
@@ -4052,12 +3944,12 @@
       </c>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
-      <c r="D187" s="21"/>
-      <c r="E187" s="20"/>
-      <c r="F187" s="20"/>
-      <c r="G187" s="20"/>
-      <c r="H187" s="20"/>
-      <c r="I187" s="20"/>
+      <c r="D187" s="19"/>
+      <c r="E187" s="18"/>
+      <c r="F187" s="18"/>
+      <c r="G187" s="18"/>
+      <c r="H187" s="18"/>
+      <c r="I187" s="18"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
@@ -4066,12 +3958,12 @@
       </c>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
-      <c r="D188" s="21"/>
-      <c r="E188" s="20"/>
-      <c r="F188" s="20"/>
-      <c r="G188" s="20"/>
-      <c r="H188" s="20"/>
-      <c r="I188" s="20"/>
+      <c r="D188" s="19"/>
+      <c r="E188" s="18"/>
+      <c r="F188" s="18"/>
+      <c r="G188" s="18"/>
+      <c r="H188" s="18"/>
+      <c r="I188" s="18"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
@@ -4080,12 +3972,12 @@
       </c>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
-      <c r="D189" s="21"/>
-      <c r="E189" s="20"/>
-      <c r="F189" s="20"/>
-      <c r="G189" s="20"/>
-      <c r="H189" s="20"/>
-      <c r="I189" s="20"/>
+      <c r="D189" s="19"/>
+      <c r="E189" s="18"/>
+      <c r="F189" s="18"/>
+      <c r="G189" s="18"/>
+      <c r="H189" s="18"/>
+      <c r="I189" s="18"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
@@ -4094,12 +3986,12 @@
       </c>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
-      <c r="D190" s="21"/>
-      <c r="E190" s="20"/>
-      <c r="F190" s="20"/>
-      <c r="G190" s="20"/>
-      <c r="H190" s="20"/>
-      <c r="I190" s="20"/>
+      <c r="D190" s="18"/>
+      <c r="E190" s="18"/>
+      <c r="F190" s="18"/>
+      <c r="G190" s="18"/>
+      <c r="H190" s="18"/>
+      <c r="I190" s="18"/>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
@@ -4108,12 +4000,12 @@
       </c>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
-      <c r="D191" s="21"/>
-      <c r="E191" s="20"/>
-      <c r="F191" s="20"/>
-      <c r="G191" s="20"/>
-      <c r="H191" s="20"/>
-      <c r="I191" s="20"/>
+      <c r="D191" s="18"/>
+      <c r="E191" s="18"/>
+      <c r="F191" s="18"/>
+      <c r="G191" s="18"/>
+      <c r="H191" s="18"/>
+      <c r="I191" s="18"/>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
@@ -4122,12 +4014,12 @@
       </c>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
-      <c r="D192" s="21"/>
-      <c r="E192" s="20"/>
-      <c r="F192" s="20"/>
-      <c r="G192" s="20"/>
-      <c r="H192" s="20"/>
-      <c r="I192" s="20"/>
+      <c r="D192" s="18"/>
+      <c r="E192" s="18"/>
+      <c r="F192" s="18"/>
+      <c r="G192" s="18"/>
+      <c r="H192" s="18"/>
+      <c r="I192" s="18"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
@@ -4136,12 +4028,12 @@
       </c>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
-      <c r="D193" s="20"/>
-      <c r="E193" s="20"/>
-      <c r="F193" s="20"/>
-      <c r="G193" s="20"/>
-      <c r="H193" s="20"/>
-      <c r="I193" s="20"/>
+      <c r="D193" s="18"/>
+      <c r="E193" s="18"/>
+      <c r="F193" s="18"/>
+      <c r="G193" s="18"/>
+      <c r="H193" s="18"/>
+      <c r="I193" s="18"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
@@ -4150,12 +4042,12 @@
       </c>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
-      <c r="D194" s="20"/>
-      <c r="E194" s="20"/>
-      <c r="F194" s="20"/>
-      <c r="G194" s="20"/>
-      <c r="H194" s="20"/>
-      <c r="I194" s="20"/>
+      <c r="D194" s="19"/>
+      <c r="E194" s="18"/>
+      <c r="F194" s="18"/>
+      <c r="G194" s="18"/>
+      <c r="H194" s="18"/>
+      <c r="I194" s="18"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
@@ -4164,12 +4056,12 @@
       </c>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
-      <c r="D195" s="20"/>
-      <c r="E195" s="20"/>
-      <c r="F195" s="20"/>
-      <c r="G195" s="20"/>
-      <c r="H195" s="20"/>
-      <c r="I195" s="20"/>
+      <c r="D195" s="19"/>
+      <c r="E195" s="18"/>
+      <c r="F195" s="18"/>
+      <c r="G195" s="18"/>
+      <c r="H195" s="18"/>
+      <c r="I195" s="18"/>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
@@ -4178,107 +4070,63 @@
       </c>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
-      <c r="D196" s="20"/>
-      <c r="E196" s="20"/>
-      <c r="F196" s="20"/>
-      <c r="G196" s="20"/>
-      <c r="H196" s="20"/>
-      <c r="I196" s="20"/>
+      <c r="D196" s="19"/>
+      <c r="E196" s="18"/>
+      <c r="F196" s="18"/>
+      <c r="G196" s="18"/>
+      <c r="H196" s="18"/>
+      <c r="I196" s="18"/>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A197" s="7">
-        <f t="shared" si="5"/>
+      <c r="A197" s="9">
+        <f t="shared" ref="A197" si="6">ROW(190:197)</f>
         <v>190</v>
       </c>
-      <c r="B197" s="8"/>
-      <c r="C197" s="8"/>
-      <c r="D197" s="21"/>
-      <c r="E197" s="20"/>
-      <c r="F197" s="20"/>
-      <c r="G197" s="20"/>
-      <c r="H197" s="20"/>
-      <c r="I197" s="20"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A198" s="7">
-        <f t="shared" si="5"/>
-        <v>191</v>
-      </c>
-      <c r="B198" s="8"/>
-      <c r="C198" s="8"/>
-      <c r="D198" s="21"/>
-      <c r="E198" s="20"/>
-      <c r="F198" s="20"/>
-      <c r="G198" s="20"/>
-      <c r="H198" s="20"/>
-      <c r="I198" s="20"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A199" s="7">
-        <f t="shared" si="5"/>
-        <v>192</v>
-      </c>
-      <c r="B199" s="8"/>
-      <c r="C199" s="8"/>
-      <c r="D199" s="21"/>
-      <c r="E199" s="20"/>
-      <c r="F199" s="20"/>
-      <c r="G199" s="20"/>
-      <c r="H199" s="20"/>
-      <c r="I199" s="20"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A200" s="9">
-        <f t="shared" ref="A200:A231" si="6">ROW(193:200)</f>
-        <v>193</v>
-      </c>
-      <c r="B200" s="10"/>
-      <c r="C200" s="10"/>
-      <c r="D200" s="22"/>
-      <c r="E200" s="20"/>
-      <c r="F200" s="20"/>
-      <c r="G200" s="20"/>
-      <c r="H200" s="20"/>
-      <c r="I200" s="20"/>
+      <c r="B197" s="10"/>
+      <c r="C197" s="10"/>
+      <c r="D197" s="20"/>
+      <c r="E197" s="18"/>
+      <c r="F197" s="18"/>
+      <c r="G197" s="18"/>
+      <c r="H197" s="18"/>
+      <c r="I197" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:I200">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>OR($C8="Select_Dropdown",$C8="Radio_Button")</formula>
+  <conditionalFormatting sqref="D5:I197">
+    <cfRule type="expression" dxfId="41" priority="5">
+      <formula>OR($C5="Select_Dropdown",$C5="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:I200">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>OR($C8="Browser_Back",$C8="Browser_Forward",$C8="Browser_Refresh",$C8="Capture_Alert",$C8="Admin_Portal_Login",$C8="Browser_Quit",$C8="SINT_Login")</formula>
+  <conditionalFormatting sqref="H5:I197">
+    <cfRule type="expression" dxfId="40" priority="4">
+      <formula>OR($C5="Browser_Back",$C5="Browser_Forward",$C5="Browser_Refresh",$C5="Capture_Alert",$C5="Admin_Portal_Login",$C5="Browser_Quit",$C5="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:F200 H8:I200">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>OR($C8="Check_Box_Data",$C8="Check_Log_File",$C8="Write_To_Editor",$C8="Write_Box_Data",$C8="Insert_Value_Config")</formula>
+  <conditionalFormatting sqref="D5:F197 H5:I197">
+    <cfRule type="expression" dxfId="39" priority="1">
+      <formula>OR($C5="Check_Box_Data",$C5="Check_Log_File",$C5="Write_To_Editor",$C5="Write_Box_Data",$C5="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:E200 H8:I200">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>OR($C8="Click_Button",$C8="Check_Box",$C8="List_All_Dropdown_Values")</formula>
+  <conditionalFormatting sqref="D5:E197 H5:I197">
+    <cfRule type="expression" dxfId="38" priority="2">
+      <formula>OR($C5="Click_Button",$C5="Check_Box",$C5="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D200 H8:I200">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>OR($C8="Portal_Login",$C8="Handle_Browser_window",$C8="Ping_Test",$C8="Open_URL",$C8="Check_URL",$C8="iPause",$C8="Check_Screen_Data",$C8="Execute_System_Command",$C8="Check_Browser_Title",$C8="Open_Portal_URL",$C8="Send_Special_keys")</formula>
+  <conditionalFormatting sqref="D5:D197 H5:I197">
+    <cfRule type="expression" dxfId="37" priority="3">
+      <formula>OR($C5="Portal_Login",$C5="Handle_Browser_window",$C5="Ping_Test",$C5="Open_URL",$C5="Check_URL",$C5="iPause",$C5="Check_Screen_Data",$C5="Execute_System_Command",$C5="Check_Browser_Title",$C5="Open_Portal_URL",$C5="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:I200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:I197">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4287,13 +4135,13 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$29</xm:f>
           </x14:formula1>
-          <xm:sqref>C8:C200</xm:sqref>
+          <xm:sqref>C5:C197</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E200 G8:G200</xm:sqref>
+          <xm:sqref>E5:E197 G5:G197</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4305,8 +4153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4318,234 +4166,226 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="17"/>
       <c r="D1" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="B2" s="12"/>
       <c r="D2" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="B3" s="12"/>
       <c r="D3" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="D4" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="D5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="D4" s="8" t="s">
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="D7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="D8" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="D10" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="D11" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="D12" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="D13" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="D14" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="D5" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="D7" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="D8" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="D9" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="D10" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="D11" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="D12" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="D14" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B21" s="13"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="B23" s="13"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="B24" s="13"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="B25" s="13"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="B26" s="13"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="15"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="B27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="15"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="A28" s="14"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="A29" s="14"/>
+      <c r="B29" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tidy up of the code
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/GitHub/TAF/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/TAF_Master/taf/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31080" windowHeight="18720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20420" yWindow="-20880" windowWidth="31080" windowHeight="18720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Spec" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Project_ID</t>
   </si>
@@ -135,6 +135,18 @@
     <t>Custom Function to login to portal</t>
   </si>
   <si>
+    <t>SINT_Login</t>
+  </si>
+  <si>
+    <t>Custom Function to login to sint</t>
+  </si>
+  <si>
+    <t>Admin_Portal_Login</t>
+  </si>
+  <si>
+    <t>Custom Function to login to Admin portal</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -199,6 +211,9 @@
   </si>
   <si>
     <t>Skip_Test_Case</t>
+  </si>
+  <si>
+    <t>visible_text</t>
   </si>
 </sst>
 </file>
@@ -425,7 +440,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1002,60 +1057,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <tableColumns count="3">
-    <tableColumn id="1" name="Test_ID" dataDxfId="32"/>
-    <tableColumn id="2" name="Project_ID" dataDxfId="31"/>
-    <tableColumn id="3" name="Test_Description" dataDxfId="30"/>
+    <tableColumn id="1" name="Test_ID" dataDxfId="36"/>
+    <tableColumn id="2" name="Project_ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Test_Description" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <tableColumns count="9">
-    <tableColumn id="1" name="Test_Step" dataDxfId="24">
+    <tableColumn id="1" name="Test_Step" dataDxfId="28">
       <calculatedColumnFormula>ROW(1:5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Test_Step_Description" dataDxfId="23"/>
-    <tableColumn id="3" name="Test_Step_Function" dataDxfId="22"/>
-    <tableColumn id="4" name="Test_Step_Value" dataDxfId="21"/>
-    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="20"/>
-    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="19"/>
-    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="18"/>
-    <tableColumn id="8" name="Screenshot" dataDxfId="17"/>
-    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="16"/>
+    <tableColumn id="2" name="Test_Step_Description" dataDxfId="27"/>
+    <tableColumn id="3" name="Test_Step_Function" dataDxfId="26"/>
+    <tableColumn id="4" name="Test_Step_Value" dataDxfId="25"/>
+    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="24"/>
+    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="23"/>
+    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="22"/>
+    <tableColumn id="8" name="Screenshot" dataDxfId="21"/>
+    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:A29"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="10"/>
+    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="D1:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="D1:D15"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Locator" dataDxfId="4"/>
+    <tableColumn id="1" name="Ruby_Locator" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="B1:B29"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" name="Notes" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1326,9 +1381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,22 +1426,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4093,27 +4148,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:I197">
-    <cfRule type="expression" dxfId="41" priority="5">
+    <cfRule type="expression" dxfId="45" priority="5">
       <formula>OR($C5="Select_Dropdown",$C5="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197">
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="44" priority="4">
       <formula>OR($C5="Browser_Back",$C5="Browser_Forward",$C5="Browser_Refresh",$C5="Capture_Alert",$C5="Admin_Portal_Login",$C5="Browser_Quit",$C5="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:F197 H5:I197">
-    <cfRule type="expression" dxfId="39" priority="1">
+  <conditionalFormatting sqref="H5:I197 D5:F197">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>OR($C5="Check_Box_Data",$C5="Check_Log_File",$C5="Write_To_Editor",$C5="Write_Box_Data",$C5="Insert_Value_Config")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:E197 H5:I197">
-    <cfRule type="expression" dxfId="38" priority="2">
+  <conditionalFormatting sqref="H5:I197 D5:E197">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>OR($C5="Click_Button",$C5="Check_Box",$C5="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D197 H5:I197">
-    <cfRule type="expression" dxfId="37" priority="3">
+    <cfRule type="expression" dxfId="41" priority="3">
       <formula>OR($C5="Portal_Login",$C5="Handle_Browser_window",$C5="Ping_Test",$C5="Open_URL",$C5="Check_URL",$C5="iPause",$C5="Check_Screen_Data",$C5="Execute_System_Command",$C5="Check_Browser_Title",$C5="Open_Portal_URL",$C5="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4139,7 +4194,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$D$2:$D$14</xm:f>
+            <xm:f>Lists!$D$2:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E197 G5:G197</xm:sqref>
         </x14:dataValidation>
@@ -4153,8 +4208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4166,14 +4221,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4182,7 +4237,7 @@
       </c>
       <c r="B2" s="12"/>
       <c r="D2" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4191,7 +4246,7 @@
       </c>
       <c r="B3" s="12"/>
       <c r="D3" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4200,7 +4255,7 @@
       </c>
       <c r="B4" s="12"/>
       <c r="D4" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4209,7 +4264,7 @@
       </c>
       <c r="B5" s="13"/>
       <c r="D5" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4220,7 +4275,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4229,7 +4284,7 @@
       </c>
       <c r="B7" s="13"/>
       <c r="D7" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4238,7 +4293,7 @@
       </c>
       <c r="B8" s="13"/>
       <c r="D8" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4247,7 +4302,7 @@
       </c>
       <c r="B9" s="13"/>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4256,7 +4311,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4265,7 +4320,7 @@
       </c>
       <c r="B11" s="13"/>
       <c r="D11" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4274,7 +4329,7 @@
       </c>
       <c r="B12" s="13"/>
       <c r="D12" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4283,7 +4338,7 @@
       </c>
       <c r="B13" s="13"/>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4292,7 +4347,7 @@
       </c>
       <c r="B14" s="13"/>
       <c r="D14" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4300,6 +4355,9 @@
         <v>20</v>
       </c>
       <c r="B15" s="13"/>
+      <c r="D15" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
@@ -4380,12 +4438,20 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated taf so some functions can use env for a string and change the gem build process to use docker
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Documents/TAF_Master/taf/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Projects/QA_Tools_new/taf/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20420" yWindow="-20880" windowWidth="31080" windowHeight="18720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31080" windowHeight="18720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Spec" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Project_ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Execute_System_Command</t>
   </si>
   <si>
-    <t>Insert_value_config</t>
-  </si>
-  <si>
     <t>iPause</t>
   </si>
   <si>
@@ -105,12 +102,6 @@
     <t>Open_URL</t>
   </si>
   <si>
-    <t>Open_Portal_URL</t>
-  </si>
-  <si>
-    <t>Custom for Portal</t>
-  </si>
-  <si>
     <t>Ping_Test</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
   </si>
   <si>
     <t>Write_Box_Data</t>
-  </si>
-  <si>
-    <t>Write_To_Editor</t>
   </si>
   <si>
     <t>Portal_Login</t>
@@ -440,7 +428,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -996,56 +1044,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1057,60 +1055,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="3">
-    <tableColumn id="1" name="Test_ID" dataDxfId="36"/>
-    <tableColumn id="2" name="Project_ID" dataDxfId="35"/>
-    <tableColumn id="3" name="Test_Description" dataDxfId="34"/>
+    <tableColumn id="1" name="Test_ID" dataDxfId="42"/>
+    <tableColumn id="2" name="Project_ID" dataDxfId="41"/>
+    <tableColumn id="3" name="Test_Description" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <tableColumns count="9">
-    <tableColumn id="1" name="Test_Step" dataDxfId="28">
+    <tableColumn id="1" name="Test_Step" dataDxfId="34">
       <calculatedColumnFormula>ROW(1:5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Test_Step_Description" dataDxfId="27"/>
-    <tableColumn id="3" name="Test_Step_Function" dataDxfId="26"/>
-    <tableColumn id="4" name="Test_Step_Value" dataDxfId="25"/>
-    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="24"/>
-    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="23"/>
-    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="22"/>
-    <tableColumn id="8" name="Screenshot" dataDxfId="21"/>
-    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="20"/>
+    <tableColumn id="2" name="Test_Step_Description" dataDxfId="33"/>
+    <tableColumn id="3" name="Test_Step_Function" dataDxfId="32"/>
+    <tableColumn id="4" name="Test_Step_Value" dataDxfId="31"/>
+    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="30"/>
+    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="29"/>
+    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="28"/>
+    <tableColumn id="8" name="Screenshot" dataDxfId="27"/>
+    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A26" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A1:A26"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="14"/>
+    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="D1:D15"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Locator" dataDxfId="8"/>
+    <tableColumn id="1" name="Ruby_Locator" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="B1:B29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="B1:B26"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Notes" dataDxfId="4"/>
+    <tableColumn id="1" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1383,7 +1381,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,22 +1424,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4148,28 +4146,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:I197">
-    <cfRule type="expression" dxfId="45" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>OR($C5="Select_Dropdown",$C5="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197">
-    <cfRule type="expression" dxfId="44" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>OR($C5="Browser_Back",$C5="Browser_Forward",$C5="Browser_Refresh",$C5="Capture_Alert",$C5="Admin_Portal_Login",$C5="Browser_Quit",$C5="SINT_Login")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197 D5:F197">
-    <cfRule type="expression" dxfId="43" priority="1">
-      <formula>OR($C5="Check_Box_Data",$C5="Check_Log_File",$C5="Write_To_Editor",$C5="Write_Box_Data",$C5="Insert_Value_Config")</formula>
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>OR($C5="Check_Box_Data",$C5="Check_Log_File",$C5="Write_Box_Data")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197 D5:E197">
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>OR($C5="Click_Button",$C5="Check_Box",$C5="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D197 H5:I197">
-    <cfRule type="expression" dxfId="41" priority="3">
-      <formula>OR($C5="Portal_Login",$C5="Handle_Browser_window",$C5="Ping_Test",$C5="Open_URL",$C5="Check_URL",$C5="iPause",$C5="Check_Screen_Data",$C5="Execute_System_Command",$C5="Check_Browser_Title",$C5="Open_Portal_URL",$C5="Send_Special_keys")</formula>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>OR($C5="Portal_Login",$C5="Handle_Browser_window",$C5="Ping_Test",$C5="Open_URL",$C5="Check_URL",$C5="iPause",$C5="Check_Screen_Data",$C5="Execute_System_Command",$C5="Check_Browser_Title",$C5="Send_Special_keys")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4188,15 +4186,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$2:$A$29</xm:f>
+            <xm:f>Lists!$D$2:$D$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C197</xm:sqref>
+          <xm:sqref>E5:E197 G5:G197</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$D$2:$D$15</xm:f>
+            <xm:f>Lists!$A$2:$A$26</xm:f>
           </x14:formula1>
-          <xm:sqref>E5:E197 G5:G197</xm:sqref>
+          <xm:sqref>C5:C197</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4206,10 +4204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4221,14 +4219,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4237,7 +4235,7 @@
       </c>
       <c r="B2" s="12"/>
       <c r="D2" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4246,7 +4244,7 @@
       </c>
       <c r="B3" s="12"/>
       <c r="D3" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4255,7 +4253,7 @@
       </c>
       <c r="B4" s="12"/>
       <c r="D4" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4264,7 +4262,7 @@
       </c>
       <c r="B5" s="13"/>
       <c r="D5" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4275,7 +4273,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4284,7 +4282,7 @@
       </c>
       <c r="B7" s="13"/>
       <c r="D7" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4293,7 +4291,7 @@
       </c>
       <c r="B8" s="13"/>
       <c r="D8" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4302,7 +4300,7 @@
       </c>
       <c r="B9" s="13"/>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4311,7 +4309,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="D10" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4320,7 +4318,7 @@
       </c>
       <c r="B11" s="13"/>
       <c r="D11" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4329,7 +4327,7 @@
       </c>
       <c r="B12" s="13"/>
       <c r="D12" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4338,7 +4336,7 @@
       </c>
       <c r="B13" s="13"/>
       <c r="D13" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4347,7 +4345,7 @@
       </c>
       <c r="B14" s="13"/>
       <c r="D14" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4356,16 +4354,14 @@
       </c>
       <c r="B15" s="13"/>
       <c r="D15" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B16" s="13"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
@@ -4389,68 +4385,48 @@
       <c r="A20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="13"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="13"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="13"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="13"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated templated and removed portal login and code tidy
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Specification_Template.xlsx
+++ b/Excel_Templates/Test_Specification_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Projects/QA_Tools_new/taf/Excel_Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aperrett/Projects/QA_Tools/taf/Excel_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Project_ID</t>
   </si>
@@ -117,24 +117,6 @@
     <t>Write_Box_Data</t>
   </si>
   <si>
-    <t>Portal_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to portal</t>
-  </si>
-  <si>
-    <t>SINT_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to sint</t>
-  </si>
-  <si>
-    <t>Admin_Portal_Login</t>
-  </si>
-  <si>
-    <t>Custom Function to login to Admin portal</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -202,6 +184,9 @@
   </si>
   <si>
     <t>visible_text</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -374,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,7 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,7 +412,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="48">
     <dxf>
       <font>
         <color theme="1"/>
@@ -472,6 +456,16 @@
     <dxf>
       <font>
         <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1055,60 +1049,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C2" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="3">
-    <tableColumn id="1" name="Test_ID" dataDxfId="42"/>
-    <tableColumn id="2" name="Project_ID" dataDxfId="41"/>
-    <tableColumn id="3" name="Test_Description" dataDxfId="40"/>
+    <tableColumn id="1" name="Test_ID" dataDxfId="43"/>
+    <tableColumn id="2" name="Project_ID" dataDxfId="42"/>
+    <tableColumn id="3" name="Test_Description" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:I197" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="9">
-    <tableColumn id="1" name="Test_Step" dataDxfId="34">
+    <tableColumn id="1" name="Test_Step" dataDxfId="35">
       <calculatedColumnFormula>ROW(1:5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Test_Step_Description" dataDxfId="33"/>
-    <tableColumn id="3" name="Test_Step_Function" dataDxfId="32"/>
-    <tableColumn id="4" name="Test_Step_Value" dataDxfId="31"/>
-    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="30"/>
-    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="29"/>
-    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="28"/>
-    <tableColumn id="8" name="Screenshot" dataDxfId="27"/>
-    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="26"/>
+    <tableColumn id="2" name="Test_Step_Description" dataDxfId="34"/>
+    <tableColumn id="3" name="Test_Step_Function" dataDxfId="33"/>
+    <tableColumn id="4" name="Test_Step_Value" dataDxfId="32"/>
+    <tableColumn id="5" name="Locator_Finder_Value" dataDxfId="31"/>
+    <tableColumn id="6" name="Test_Step_Value2" dataDxfId="30"/>
+    <tableColumn id="7" name="Locator_Finder_Value2" dataDxfId="29"/>
+    <tableColumn id="8" name="Screenshot" dataDxfId="28"/>
+    <tableColumn id="9" name="Skip_Test_Case" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A26" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A1:A26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A24" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:A24"/>
+  <sortState ref="A2:A24">
+    <sortCondition ref="A1:A24"/>
+  </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="20"/>
+    <tableColumn id="1" name="Ruby_Web_Functions" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D1:D15" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="D1:D15"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ruby_Locator" dataDxfId="14"/>
+    <tableColumn id="1" name="Ruby_Locator" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="B1:B26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:B24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="B1:B24"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" name="Notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1381,7 +1378,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,22 +1421,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1449,12 +1446,12 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1463,12 +1460,12 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1477,12 +1474,12 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -1491,12 +1488,12 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -1505,12 +1502,12 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -1519,12 +1516,12 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
@@ -1533,12 +1530,12 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -1547,12 +1544,12 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
@@ -1561,12 +1558,12 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -1575,12 +1572,12 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -1589,12 +1586,12 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1603,12 +1600,12 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1617,12 +1614,12 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1631,12 +1628,12 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -1645,12 +1642,12 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1659,12 +1656,12 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1673,12 +1670,12 @@
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1687,12 +1684,12 @@
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -1701,12 +1698,12 @@
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1715,12 +1712,12 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
@@ -1729,12 +1726,12 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -1743,12 +1740,12 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
@@ -1757,12 +1754,12 @@
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
@@ -1771,12 +1768,12 @@
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
@@ -1785,12 +1782,12 @@
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
@@ -1799,12 +1796,12 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
@@ -1813,12 +1810,12 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
@@ -1827,12 +1824,12 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
@@ -1841,12 +1838,12 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
@@ -1855,12 +1852,12 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
@@ -1869,12 +1866,12 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
@@ -1883,12 +1880,12 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
@@ -1897,12 +1894,12 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
@@ -1911,12 +1908,12 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
@@ -1925,12 +1922,12 @@
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
@@ -1939,12 +1936,12 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -1953,12 +1950,12 @@
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
@@ -1967,12 +1964,12 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
@@ -1981,12 +1978,12 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -1995,12 +1992,12 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
@@ -2009,12 +2006,12 @@
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
@@ -2023,12 +2020,12 @@
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
@@ -2037,12 +2034,12 @@
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
@@ -2051,12 +2048,12 @@
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
@@ -2065,12 +2062,12 @@
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
@@ -2079,12 +2076,12 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
@@ -2093,12 +2090,12 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
@@ -2107,12 +2104,12 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
@@ -2121,12 +2118,12 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
@@ -2135,12 +2132,12 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
@@ -2149,12 +2146,12 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
@@ -2163,12 +2160,12 @@
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
@@ -2177,12 +2174,12 @@
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
@@ -2191,12 +2188,12 @@
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
@@ -2205,12 +2202,12 @@
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
@@ -2219,12 +2216,12 @@
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
@@ -2233,12 +2230,12 @@
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
@@ -2247,12 +2244,12 @@
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
@@ -2261,12 +2258,12 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
@@ -2275,12 +2272,12 @@
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
@@ -2289,12 +2286,12 @@
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
@@ -2303,12 +2300,12 @@
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
@@ -2317,12 +2314,12 @@
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
@@ -2331,12 +2328,12 @@
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
@@ -2345,12 +2342,12 @@
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
@@ -2359,12 +2356,12 @@
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
@@ -2373,12 +2370,12 @@
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
@@ -2387,12 +2384,12 @@
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
@@ -2401,12 +2398,12 @@
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -2415,12 +2412,12 @@
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -2429,12 +2426,12 @@
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
@@ -2443,12 +2440,12 @@
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -2457,12 +2454,12 @@
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -2471,12 +2468,12 @@
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -2485,12 +2482,12 @@
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -2499,12 +2496,12 @@
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
@@ -2513,12 +2510,12 @@
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
@@ -2527,12 +2524,12 @@
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
@@ -2541,12 +2538,12 @@
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
@@ -2555,12 +2552,12 @@
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
@@ -2569,12 +2566,12 @@
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
@@ -2583,12 +2580,12 @@
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
@@ -2597,12 +2594,12 @@
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
@@ -2611,12 +2608,12 @@
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
@@ -2625,12 +2622,12 @@
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
@@ -2639,12 +2636,12 @@
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
@@ -2653,12 +2650,12 @@
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
@@ -2667,12 +2664,12 @@
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
@@ -2681,12 +2678,12 @@
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
@@ -2695,12 +2692,12 @@
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
@@ -2709,12 +2706,12 @@
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
@@ -2723,12 +2720,12 @@
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
@@ -2737,12 +2734,12 @@
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -2751,12 +2748,12 @@
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
@@ -2765,12 +2762,12 @@
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
-      <c r="H99" s="18"/>
-      <c r="I99" s="18"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
@@ -2779,12 +2776,12 @@
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
@@ -2793,12 +2790,12 @@
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
@@ -2807,12 +2804,12 @@
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
@@ -2821,12 +2818,12 @@
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
@@ -2835,12 +2832,12 @@
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -2849,12 +2846,12 @@
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="17"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="17"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
@@ -2863,12 +2860,12 @@
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -2877,12 +2874,12 @@
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="18"/>
-      <c r="H107" s="18"/>
-      <c r="I107" s="18"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
+      <c r="I107" s="17"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -2891,12 +2888,12 @@
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
-      <c r="H108" s="18"/>
-      <c r="I108" s="18"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="17"/>
+      <c r="H108" s="17"/>
+      <c r="I108" s="17"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -2905,12 +2902,12 @@
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
-      <c r="D109" s="18"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="18"/>
-      <c r="H109" s="18"/>
-      <c r="I109" s="18"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="17"/>
+      <c r="H109" s="17"/>
+      <c r="I109" s="17"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -2919,12 +2916,12 @@
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="18"/>
-      <c r="H110" s="18"/>
-      <c r="I110" s="18"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="17"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="17"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
@@ -2933,12 +2930,12 @@
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="18"/>
-      <c r="H111" s="18"/>
-      <c r="I111" s="18"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="17"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
@@ -2947,12 +2944,12 @@
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="18"/>
-      <c r="G112" s="18"/>
-      <c r="H112" s="18"/>
-      <c r="I112" s="18"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
@@ -2961,12 +2958,12 @@
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
-      <c r="H113" s="18"/>
-      <c r="I113" s="18"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17"/>
+      <c r="I113" s="17"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
@@ -2975,12 +2972,12 @@
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
@@ -2989,12 +2986,12 @@
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
-      <c r="D115" s="18"/>
-      <c r="E115" s="18"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="18"/>
-      <c r="H115" s="18"/>
-      <c r="I115" s="18"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="17"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
@@ -3003,12 +3000,12 @@
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="18"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="18"/>
-      <c r="I116" s="18"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="17"/>
+      <c r="I116" s="17"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
@@ -3017,12 +3014,12 @@
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="18"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="18"/>
-      <c r="H117" s="18"/>
-      <c r="I117" s="18"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="17"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
@@ -3031,12 +3028,12 @@
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
-      <c r="D118" s="18"/>
-      <c r="E118" s="18"/>
-      <c r="F118" s="18"/>
-      <c r="G118" s="18"/>
-      <c r="H118" s="18"/>
-      <c r="I118" s="18"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="17"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
@@ -3045,12 +3042,12 @@
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
-      <c r="D119" s="18"/>
-      <c r="E119" s="18"/>
-      <c r="F119" s="18"/>
-      <c r="G119" s="18"/>
-      <c r="H119" s="18"/>
-      <c r="I119" s="18"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17"/>
+      <c r="I119" s="17"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
@@ -3059,12 +3056,12 @@
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="18"/>
-      <c r="F120" s="18"/>
-      <c r="G120" s="18"/>
-      <c r="H120" s="18"/>
-      <c r="I120" s="18"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
@@ -3073,12 +3070,12 @@
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
-      <c r="D121" s="18"/>
-      <c r="E121" s="18"/>
-      <c r="F121" s="18"/>
-      <c r="G121" s="18"/>
-      <c r="H121" s="18"/>
-      <c r="I121" s="18"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
@@ -3087,12 +3084,12 @@
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
-      <c r="D122" s="18"/>
-      <c r="E122" s="18"/>
-      <c r="F122" s="18"/>
-      <c r="G122" s="18"/>
-      <c r="H122" s="18"/>
-      <c r="I122" s="18"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17"/>
+      <c r="H122" s="17"/>
+      <c r="I122" s="17"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
@@ -3101,12 +3098,12 @@
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
-      <c r="D123" s="18"/>
-      <c r="E123" s="18"/>
-      <c r="F123" s="18"/>
-      <c r="G123" s="18"/>
-      <c r="H123" s="18"/>
-      <c r="I123" s="18"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="17"/>
+      <c r="G123" s="17"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="17"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
@@ -3115,12 +3112,12 @@
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
-      <c r="D124" s="18"/>
-      <c r="E124" s="18"/>
-      <c r="F124" s="18"/>
-      <c r="G124" s="18"/>
-      <c r="H124" s="18"/>
-      <c r="I124" s="18"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="17"/>
+      <c r="G124" s="17"/>
+      <c r="H124" s="17"/>
+      <c r="I124" s="17"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
@@ -3129,12 +3126,12 @@
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
-      <c r="D125" s="18"/>
-      <c r="E125" s="18"/>
-      <c r="F125" s="18"/>
-      <c r="G125" s="18"/>
-      <c r="H125" s="18"/>
-      <c r="I125" s="18"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="17"/>
+      <c r="G125" s="17"/>
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
@@ -3143,12 +3140,12 @@
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
-      <c r="D126" s="18"/>
-      <c r="E126" s="18"/>
-      <c r="F126" s="18"/>
-      <c r="G126" s="18"/>
-      <c r="H126" s="18"/>
-      <c r="I126" s="18"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="17"/>
+      <c r="G126" s="17"/>
+      <c r="H126" s="17"/>
+      <c r="I126" s="17"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
@@ -3157,12 +3154,12 @@
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
-      <c r="D127" s="18"/>
-      <c r="E127" s="18"/>
-      <c r="F127" s="18"/>
-      <c r="G127" s="18"/>
-      <c r="H127" s="18"/>
-      <c r="I127" s="18"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="17"/>
+      <c r="G127" s="17"/>
+      <c r="H127" s="17"/>
+      <c r="I127" s="17"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
@@ -3171,12 +3168,12 @@
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
-      <c r="D128" s="18"/>
-      <c r="E128" s="18"/>
-      <c r="F128" s="18"/>
-      <c r="G128" s="18"/>
-      <c r="H128" s="18"/>
-      <c r="I128" s="18"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="17"/>
+      <c r="G128" s="17"/>
+      <c r="H128" s="17"/>
+      <c r="I128" s="17"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
@@ -3185,12 +3182,12 @@
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
-      <c r="D129" s="18"/>
-      <c r="E129" s="18"/>
-      <c r="F129" s="18"/>
-      <c r="G129" s="18"/>
-      <c r="H129" s="18"/>
-      <c r="I129" s="18"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="17"/>
+      <c r="G129" s="17"/>
+      <c r="H129" s="17"/>
+      <c r="I129" s="17"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -3199,12 +3196,12 @@
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="18"/>
-      <c r="E130" s="18"/>
-      <c r="F130" s="18"/>
-      <c r="G130" s="18"/>
-      <c r="H130" s="18"/>
-      <c r="I130" s="18"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -3213,12 +3210,12 @@
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="18"/>
-      <c r="F131" s="18"/>
-      <c r="G131" s="18"/>
-      <c r="H131" s="18"/>
-      <c r="I131" s="18"/>
+      <c r="D131" s="18"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="17"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="17"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="7">
@@ -3227,12 +3224,12 @@
       </c>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="18"/>
-      <c r="F132" s="18"/>
-      <c r="G132" s="18"/>
-      <c r="H132" s="18"/>
-      <c r="I132" s="18"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="17"/>
+      <c r="G132" s="17"/>
+      <c r="H132" s="17"/>
+      <c r="I132" s="17"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
@@ -3241,12 +3238,12 @@
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
-      <c r="D133" s="19"/>
-      <c r="E133" s="18"/>
-      <c r="F133" s="18"/>
-      <c r="G133" s="18"/>
-      <c r="H133" s="18"/>
-      <c r="I133" s="18"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+      <c r="G133" s="17"/>
+      <c r="H133" s="17"/>
+      <c r="I133" s="17"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
@@ -3255,12 +3252,12 @@
       </c>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
-      <c r="D134" s="19"/>
-      <c r="E134" s="18"/>
-      <c r="F134" s="18"/>
-      <c r="G134" s="18"/>
-      <c r="H134" s="18"/>
-      <c r="I134" s="18"/>
+      <c r="D134" s="18"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="17"/>
+      <c r="H134" s="17"/>
+      <c r="I134" s="17"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
@@ -3269,12 +3266,12 @@
       </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
-      <c r="D135" s="19"/>
-      <c r="E135" s="18"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
-      <c r="I135" s="18"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="17"/>
+      <c r="H135" s="17"/>
+      <c r="I135" s="17"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
@@ -3283,12 +3280,12 @@
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
-      <c r="D136" s="19"/>
-      <c r="E136" s="18"/>
-      <c r="F136" s="18"/>
-      <c r="G136" s="18"/>
-      <c r="H136" s="18"/>
-      <c r="I136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="17"/>
+      <c r="G136" s="17"/>
+      <c r="H136" s="17"/>
+      <c r="I136" s="17"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
@@ -3297,12 +3294,12 @@
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
-      <c r="D137" s="19"/>
-      <c r="E137" s="18"/>
-      <c r="F137" s="18"/>
-      <c r="G137" s="18"/>
-      <c r="H137" s="18"/>
-      <c r="I137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="17"/>
+      <c r="H137" s="17"/>
+      <c r="I137" s="17"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
@@ -3311,12 +3308,12 @@
       </c>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
-      <c r="D138" s="19"/>
-      <c r="E138" s="18"/>
-      <c r="F138" s="18"/>
-      <c r="G138" s="18"/>
-      <c r="H138" s="18"/>
-      <c r="I138" s="18"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="17"/>
+      <c r="I138" s="17"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
@@ -3325,12 +3322,12 @@
       </c>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
-      <c r="D139" s="19"/>
-      <c r="E139" s="18"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="18"/>
-      <c r="H139" s="18"/>
-      <c r="I139" s="18"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="17"/>
+      <c r="I139" s="17"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
@@ -3339,12 +3336,12 @@
       </c>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="19"/>
-      <c r="E140" s="18"/>
-      <c r="F140" s="18"/>
-      <c r="G140" s="18"/>
-      <c r="H140" s="18"/>
-      <c r="I140" s="18"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="17"/>
+      <c r="G140" s="17"/>
+      <c r="H140" s="17"/>
+      <c r="I140" s="17"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
@@ -3353,12 +3350,12 @@
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
-      <c r="D141" s="19"/>
-      <c r="E141" s="18"/>
-      <c r="F141" s="18"/>
-      <c r="G141" s="18"/>
-      <c r="H141" s="18"/>
-      <c r="I141" s="18"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="17"/>
+      <c r="F141" s="17"/>
+      <c r="G141" s="17"/>
+      <c r="H141" s="17"/>
+      <c r="I141" s="17"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
@@ -3367,12 +3364,12 @@
       </c>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
-      <c r="D142" s="19"/>
-      <c r="E142" s="18"/>
-      <c r="F142" s="18"/>
-      <c r="G142" s="18"/>
-      <c r="H142" s="18"/>
-      <c r="I142" s="18"/>
+      <c r="D142" s="18"/>
+      <c r="E142" s="17"/>
+      <c r="F142" s="17"/>
+      <c r="G142" s="17"/>
+      <c r="H142" s="17"/>
+      <c r="I142" s="17"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
@@ -3381,12 +3378,12 @@
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
-      <c r="D143" s="19"/>
-      <c r="E143" s="18"/>
-      <c r="F143" s="18"/>
-      <c r="G143" s="18"/>
-      <c r="H143" s="18"/>
-      <c r="I143" s="18"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="17"/>
+      <c r="G143" s="17"/>
+      <c r="H143" s="17"/>
+      <c r="I143" s="17"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
@@ -3395,12 +3392,12 @@
       </c>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
-      <c r="D144" s="19"/>
-      <c r="E144" s="18"/>
-      <c r="F144" s="18"/>
-      <c r="G144" s="18"/>
-      <c r="H144" s="18"/>
-      <c r="I144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="17"/>
+      <c r="G144" s="17"/>
+      <c r="H144" s="17"/>
+      <c r="I144" s="17"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
@@ -3409,12 +3406,12 @@
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
-      <c r="D145" s="19"/>
-      <c r="E145" s="18"/>
-      <c r="F145" s="18"/>
-      <c r="G145" s="18"/>
-      <c r="H145" s="18"/>
-      <c r="I145" s="18"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="17"/>
+      <c r="G145" s="17"/>
+      <c r="H145" s="17"/>
+      <c r="I145" s="17"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
@@ -3423,12 +3420,12 @@
       </c>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
-      <c r="D146" s="19"/>
-      <c r="E146" s="18"/>
-      <c r="F146" s="18"/>
-      <c r="G146" s="18"/>
-      <c r="H146" s="18"/>
-      <c r="I146" s="18"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="17"/>
+      <c r="G146" s="17"/>
+      <c r="H146" s="17"/>
+      <c r="I146" s="17"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
@@ -3437,12 +3434,12 @@
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
-      <c r="D147" s="19"/>
-      <c r="E147" s="18"/>
-      <c r="F147" s="18"/>
-      <c r="G147" s="18"/>
-      <c r="H147" s="18"/>
-      <c r="I147" s="18"/>
+      <c r="D147" s="18"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="17"/>
+      <c r="H147" s="17"/>
+      <c r="I147" s="17"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
@@ -3451,12 +3448,12 @@
       </c>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
-      <c r="D148" s="19"/>
-      <c r="E148" s="18"/>
-      <c r="F148" s="18"/>
-      <c r="G148" s="18"/>
-      <c r="H148" s="18"/>
-      <c r="I148" s="18"/>
+      <c r="D148" s="18"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="17"/>
+      <c r="I148" s="17"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
@@ -3465,12 +3462,12 @@
       </c>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
-      <c r="D149" s="19"/>
-      <c r="E149" s="18"/>
-      <c r="F149" s="18"/>
-      <c r="G149" s="18"/>
-      <c r="H149" s="18"/>
-      <c r="I149" s="18"/>
+      <c r="D149" s="18"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17"/>
+      <c r="G149" s="17"/>
+      <c r="H149" s="17"/>
+      <c r="I149" s="17"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
@@ -3479,12 +3476,12 @@
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
-      <c r="D150" s="18"/>
-      <c r="E150" s="18"/>
-      <c r="F150" s="18"/>
-      <c r="G150" s="18"/>
-      <c r="H150" s="18"/>
-      <c r="I150" s="18"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+      <c r="G150" s="17"/>
+      <c r="H150" s="17"/>
+      <c r="I150" s="17"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
@@ -3493,12 +3490,12 @@
       </c>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
-      <c r="D151" s="18"/>
-      <c r="E151" s="18"/>
-      <c r="F151" s="18"/>
-      <c r="G151" s="18"/>
-      <c r="H151" s="18"/>
-      <c r="I151" s="18"/>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="17"/>
+      <c r="G151" s="17"/>
+      <c r="H151" s="17"/>
+      <c r="I151" s="17"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
@@ -3507,12 +3504,12 @@
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
-      <c r="D152" s="18"/>
-      <c r="E152" s="18"/>
-      <c r="F152" s="18"/>
-      <c r="G152" s="18"/>
-      <c r="H152" s="18"/>
-      <c r="I152" s="18"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="17"/>
+      <c r="G152" s="17"/>
+      <c r="H152" s="17"/>
+      <c r="I152" s="17"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
@@ -3521,12 +3518,12 @@
       </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
-      <c r="D153" s="18"/>
-      <c r="E153" s="18"/>
-      <c r="F153" s="18"/>
-      <c r="G153" s="18"/>
-      <c r="H153" s="18"/>
-      <c r="I153" s="18"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="17"/>
+      <c r="G153" s="17"/>
+      <c r="H153" s="17"/>
+      <c r="I153" s="17"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
@@ -3535,12 +3532,12 @@
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
-      <c r="D154" s="18"/>
-      <c r="E154" s="18"/>
-      <c r="F154" s="18"/>
-      <c r="G154" s="18"/>
-      <c r="H154" s="18"/>
-      <c r="I154" s="18"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="17"/>
+      <c r="G154" s="17"/>
+      <c r="H154" s="17"/>
+      <c r="I154" s="17"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
@@ -3549,12 +3546,12 @@
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
-      <c r="D155" s="18"/>
-      <c r="E155" s="18"/>
-      <c r="F155" s="18"/>
-      <c r="G155" s="18"/>
-      <c r="H155" s="18"/>
-      <c r="I155" s="18"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="17"/>
+      <c r="G155" s="17"/>
+      <c r="H155" s="17"/>
+      <c r="I155" s="17"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
@@ -3563,12 +3560,12 @@
       </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
-      <c r="D156" s="18"/>
-      <c r="E156" s="18"/>
-      <c r="F156" s="18"/>
-      <c r="G156" s="18"/>
-      <c r="H156" s="18"/>
-      <c r="I156" s="18"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="17"/>
+      <c r="G156" s="17"/>
+      <c r="H156" s="17"/>
+      <c r="I156" s="17"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
@@ -3577,12 +3574,12 @@
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
-      <c r="D157" s="18"/>
-      <c r="E157" s="18"/>
-      <c r="F157" s="18"/>
-      <c r="G157" s="18"/>
-      <c r="H157" s="18"/>
-      <c r="I157" s="18"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="17"/>
+      <c r="G157" s="17"/>
+      <c r="H157" s="17"/>
+      <c r="I157" s="17"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
@@ -3591,12 +3588,12 @@
       </c>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
-      <c r="D158" s="18"/>
-      <c r="E158" s="18"/>
-      <c r="F158" s="18"/>
-      <c r="G158" s="18"/>
-      <c r="H158" s="18"/>
-      <c r="I158" s="18"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17"/>
+      <c r="G158" s="17"/>
+      <c r="H158" s="17"/>
+      <c r="I158" s="17"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
@@ -3605,12 +3602,12 @@
       </c>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
-      <c r="D159" s="18"/>
-      <c r="E159" s="18"/>
-      <c r="F159" s="18"/>
-      <c r="G159" s="18"/>
-      <c r="H159" s="18"/>
-      <c r="I159" s="18"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="17"/>
+      <c r="I159" s="17"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
@@ -3619,12 +3616,12 @@
       </c>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
-      <c r="D160" s="18"/>
-      <c r="E160" s="18"/>
-      <c r="F160" s="18"/>
-      <c r="G160" s="18"/>
-      <c r="H160" s="18"/>
-      <c r="I160" s="18"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17"/>
+      <c r="G160" s="17"/>
+      <c r="H160" s="17"/>
+      <c r="I160" s="17"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
@@ -3633,12 +3630,12 @@
       </c>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
-      <c r="D161" s="18"/>
-      <c r="E161" s="18"/>
-      <c r="F161" s="18"/>
-      <c r="G161" s="18"/>
-      <c r="H161" s="18"/>
-      <c r="I161" s="18"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
+      <c r="G161" s="17"/>
+      <c r="H161" s="17"/>
+      <c r="I161" s="17"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
@@ -3647,12 +3644,12 @@
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
-      <c r="D162" s="18"/>
-      <c r="E162" s="18"/>
-      <c r="F162" s="18"/>
-      <c r="G162" s="18"/>
-      <c r="H162" s="18"/>
-      <c r="I162" s="18"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="17"/>
+      <c r="H162" s="17"/>
+      <c r="I162" s="17"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
@@ -3661,12 +3658,12 @@
       </c>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
-      <c r="D163" s="18"/>
-      <c r="E163" s="18"/>
-      <c r="F163" s="18"/>
-      <c r="G163" s="18"/>
-      <c r="H163" s="18"/>
-      <c r="I163" s="18"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="17"/>
+      <c r="H163" s="17"/>
+      <c r="I163" s="17"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
@@ -3675,12 +3672,12 @@
       </c>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
-      <c r="D164" s="18"/>
-      <c r="E164" s="18"/>
-      <c r="F164" s="18"/>
-      <c r="G164" s="18"/>
-      <c r="H164" s="18"/>
-      <c r="I164" s="18"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="17"/>
+      <c r="G164" s="17"/>
+      <c r="H164" s="17"/>
+      <c r="I164" s="17"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
@@ -3689,12 +3686,12 @@
       </c>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
-      <c r="D165" s="18"/>
-      <c r="E165" s="18"/>
-      <c r="F165" s="18"/>
-      <c r="G165" s="18"/>
-      <c r="H165" s="18"/>
-      <c r="I165" s="18"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="17"/>
+      <c r="F165" s="17"/>
+      <c r="G165" s="17"/>
+      <c r="H165" s="17"/>
+      <c r="I165" s="17"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
@@ -3703,12 +3700,12 @@
       </c>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
-      <c r="D166" s="18"/>
-      <c r="E166" s="18"/>
-      <c r="F166" s="18"/>
-      <c r="G166" s="18"/>
-      <c r="H166" s="18"/>
-      <c r="I166" s="18"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="17"/>
+      <c r="G166" s="17"/>
+      <c r="H166" s="17"/>
+      <c r="I166" s="17"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
@@ -3717,12 +3714,12 @@
       </c>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
-      <c r="D167" s="18"/>
-      <c r="E167" s="18"/>
-      <c r="F167" s="18"/>
-      <c r="G167" s="18"/>
-      <c r="H167" s="18"/>
-      <c r="I167" s="18"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="17"/>
+      <c r="G167" s="17"/>
+      <c r="H167" s="17"/>
+      <c r="I167" s="17"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
@@ -3731,12 +3728,12 @@
       </c>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
-      <c r="D168" s="18"/>
-      <c r="E168" s="18"/>
-      <c r="F168" s="18"/>
-      <c r="G168" s="18"/>
-      <c r="H168" s="18"/>
-      <c r="I168" s="18"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="17"/>
+      <c r="G168" s="17"/>
+      <c r="H168" s="17"/>
+      <c r="I168" s="17"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
@@ -3745,12 +3742,12 @@
       </c>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
-      <c r="D169" s="18"/>
-      <c r="E169" s="18"/>
-      <c r="F169" s="18"/>
-      <c r="G169" s="18"/>
-      <c r="H169" s="18"/>
-      <c r="I169" s="18"/>
+      <c r="D169" s="17"/>
+      <c r="E169" s="17"/>
+      <c r="F169" s="17"/>
+      <c r="G169" s="17"/>
+      <c r="H169" s="17"/>
+      <c r="I169" s="17"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
@@ -3759,12 +3756,12 @@
       </c>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
-      <c r="D170" s="18"/>
-      <c r="E170" s="18"/>
-      <c r="F170" s="18"/>
-      <c r="G170" s="18"/>
-      <c r="H170" s="18"/>
-      <c r="I170" s="18"/>
+      <c r="D170" s="17"/>
+      <c r="E170" s="17"/>
+      <c r="F170" s="17"/>
+      <c r="G170" s="17"/>
+      <c r="H170" s="17"/>
+      <c r="I170" s="17"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
@@ -3773,12 +3770,12 @@
       </c>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
-      <c r="D171" s="18"/>
-      <c r="E171" s="18"/>
-      <c r="F171" s="18"/>
-      <c r="G171" s="18"/>
-      <c r="H171" s="18"/>
-      <c r="I171" s="18"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="17"/>
+      <c r="H171" s="17"/>
+      <c r="I171" s="17"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
@@ -3787,12 +3784,12 @@
       </c>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
-      <c r="D172" s="19"/>
-      <c r="E172" s="18"/>
-      <c r="F172" s="18"/>
-      <c r="G172" s="18"/>
-      <c r="H172" s="18"/>
-      <c r="I172" s="18"/>
+      <c r="D172" s="18"/>
+      <c r="E172" s="17"/>
+      <c r="F172" s="17"/>
+      <c r="G172" s="17"/>
+      <c r="H172" s="17"/>
+      <c r="I172" s="17"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
@@ -3801,12 +3798,12 @@
       </c>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
-      <c r="D173" s="19"/>
-      <c r="E173" s="18"/>
-      <c r="F173" s="18"/>
-      <c r="G173" s="18"/>
-      <c r="H173" s="18"/>
-      <c r="I173" s="18"/>
+      <c r="D173" s="18"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="17"/>
+      <c r="H173" s="17"/>
+      <c r="I173" s="17"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
@@ -3815,12 +3812,12 @@
       </c>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
-      <c r="D174" s="19"/>
-      <c r="E174" s="18"/>
-      <c r="F174" s="18"/>
-      <c r="G174" s="18"/>
-      <c r="H174" s="18"/>
-      <c r="I174" s="18"/>
+      <c r="D174" s="18"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="17"/>
+      <c r="G174" s="17"/>
+      <c r="H174" s="17"/>
+      <c r="I174" s="17"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
@@ -3829,12 +3826,12 @@
       </c>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
-      <c r="D175" s="19"/>
-      <c r="E175" s="18"/>
-      <c r="F175" s="18"/>
-      <c r="G175" s="18"/>
-      <c r="H175" s="18"/>
-      <c r="I175" s="18"/>
+      <c r="D175" s="18"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="17"/>
+      <c r="G175" s="17"/>
+      <c r="H175" s="17"/>
+      <c r="I175" s="17"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
@@ -3843,12 +3840,12 @@
       </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
-      <c r="D176" s="19"/>
-      <c r="E176" s="18"/>
-      <c r="F176" s="18"/>
-      <c r="G176" s="18"/>
-      <c r="H176" s="18"/>
-      <c r="I176" s="18"/>
+      <c r="D176" s="18"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="17"/>
+      <c r="G176" s="17"/>
+      <c r="H176" s="17"/>
+      <c r="I176" s="17"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
@@ -3857,12 +3854,12 @@
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="19"/>
-      <c r="E177" s="18"/>
-      <c r="F177" s="18"/>
-      <c r="G177" s="18"/>
-      <c r="H177" s="18"/>
-      <c r="I177" s="18"/>
+      <c r="D177" s="18"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="17"/>
+      <c r="I177" s="17"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
@@ -3871,12 +3868,12 @@
       </c>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="19"/>
-      <c r="E178" s="18"/>
-      <c r="F178" s="18"/>
-      <c r="G178" s="18"/>
-      <c r="H178" s="18"/>
-      <c r="I178" s="18"/>
+      <c r="D178" s="18"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
+      <c r="I178" s="17"/>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
@@ -3885,12 +3882,12 @@
       </c>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
-      <c r="D179" s="19"/>
-      <c r="E179" s="18"/>
-      <c r="F179" s="18"/>
-      <c r="G179" s="18"/>
-      <c r="H179" s="18"/>
-      <c r="I179" s="18"/>
+      <c r="D179" s="18"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="17"/>
+      <c r="G179" s="17"/>
+      <c r="H179" s="17"/>
+      <c r="I179" s="17"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
@@ -3899,12 +3896,12 @@
       </c>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
-      <c r="D180" s="19"/>
-      <c r="E180" s="18"/>
-      <c r="F180" s="18"/>
-      <c r="G180" s="18"/>
-      <c r="H180" s="18"/>
-      <c r="I180" s="18"/>
+      <c r="D180" s="18"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="17"/>
+      <c r="G180" s="17"/>
+      <c r="H180" s="17"/>
+      <c r="I180" s="17"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
@@ -3913,12 +3910,12 @@
       </c>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
-      <c r="D181" s="19"/>
-      <c r="E181" s="18"/>
-      <c r="F181" s="18"/>
-      <c r="G181" s="18"/>
-      <c r="H181" s="18"/>
-      <c r="I181" s="18"/>
+      <c r="D181" s="18"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="17"/>
+      <c r="G181" s="17"/>
+      <c r="H181" s="17"/>
+      <c r="I181" s="17"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
@@ -3927,12 +3924,12 @@
       </c>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
-      <c r="D182" s="19"/>
-      <c r="E182" s="18"/>
-      <c r="F182" s="18"/>
-      <c r="G182" s="18"/>
-      <c r="H182" s="18"/>
-      <c r="I182" s="18"/>
+      <c r="D182" s="18"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="17"/>
+      <c r="G182" s="17"/>
+      <c r="H182" s="17"/>
+      <c r="I182" s="17"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
@@ -3941,12 +3938,12 @@
       </c>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
-      <c r="D183" s="19"/>
-      <c r="E183" s="18"/>
-      <c r="F183" s="18"/>
-      <c r="G183" s="18"/>
-      <c r="H183" s="18"/>
-      <c r="I183" s="18"/>
+      <c r="D183" s="18"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="17"/>
+      <c r="G183" s="17"/>
+      <c r="H183" s="17"/>
+      <c r="I183" s="17"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
@@ -3955,12 +3952,12 @@
       </c>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
-      <c r="D184" s="19"/>
-      <c r="E184" s="18"/>
-      <c r="F184" s="18"/>
-      <c r="G184" s="18"/>
-      <c r="H184" s="18"/>
-      <c r="I184" s="18"/>
+      <c r="D184" s="18"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+      <c r="G184" s="17"/>
+      <c r="H184" s="17"/>
+      <c r="I184" s="17"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
@@ -3969,12 +3966,12 @@
       </c>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
-      <c r="D185" s="19"/>
-      <c r="E185" s="18"/>
-      <c r="F185" s="18"/>
-      <c r="G185" s="18"/>
-      <c r="H185" s="18"/>
-      <c r="I185" s="18"/>
+      <c r="D185" s="18"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="17"/>
+      <c r="G185" s="17"/>
+      <c r="H185" s="17"/>
+      <c r="I185" s="17"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
@@ -3983,12 +3980,12 @@
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
-      <c r="D186" s="19"/>
-      <c r="E186" s="18"/>
-      <c r="F186" s="18"/>
-      <c r="G186" s="18"/>
-      <c r="H186" s="18"/>
-      <c r="I186" s="18"/>
+      <c r="D186" s="18"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="17"/>
+      <c r="G186" s="17"/>
+      <c r="H186" s="17"/>
+      <c r="I186" s="17"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
@@ -3997,12 +3994,12 @@
       </c>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
-      <c r="D187" s="19"/>
-      <c r="E187" s="18"/>
-      <c r="F187" s="18"/>
-      <c r="G187" s="18"/>
-      <c r="H187" s="18"/>
-      <c r="I187" s="18"/>
+      <c r="D187" s="18"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="17"/>
+      <c r="G187" s="17"/>
+      <c r="H187" s="17"/>
+      <c r="I187" s="17"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
@@ -4011,12 +4008,12 @@
       </c>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
-      <c r="D188" s="19"/>
-      <c r="E188" s="18"/>
-      <c r="F188" s="18"/>
-      <c r="G188" s="18"/>
-      <c r="H188" s="18"/>
-      <c r="I188" s="18"/>
+      <c r="D188" s="18"/>
+      <c r="E188" s="17"/>
+      <c r="F188" s="17"/>
+      <c r="G188" s="17"/>
+      <c r="H188" s="17"/>
+      <c r="I188" s="17"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
@@ -4025,12 +4022,12 @@
       </c>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
-      <c r="D189" s="19"/>
-      <c r="E189" s="18"/>
-      <c r="F189" s="18"/>
-      <c r="G189" s="18"/>
-      <c r="H189" s="18"/>
-      <c r="I189" s="18"/>
+      <c r="D189" s="18"/>
+      <c r="E189" s="17"/>
+      <c r="F189" s="17"/>
+      <c r="G189" s="17"/>
+      <c r="H189" s="17"/>
+      <c r="I189" s="17"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
@@ -4039,12 +4036,12 @@
       </c>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
-      <c r="D190" s="18"/>
-      <c r="E190" s="18"/>
-      <c r="F190" s="18"/>
-      <c r="G190" s="18"/>
-      <c r="H190" s="18"/>
-      <c r="I190" s="18"/>
+      <c r="D190" s="17"/>
+      <c r="E190" s="17"/>
+      <c r="F190" s="17"/>
+      <c r="G190" s="17"/>
+      <c r="H190" s="17"/>
+      <c r="I190" s="17"/>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
@@ -4053,12 +4050,12 @@
       </c>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
-      <c r="D191" s="18"/>
-      <c r="E191" s="18"/>
-      <c r="F191" s="18"/>
-      <c r="G191" s="18"/>
-      <c r="H191" s="18"/>
-      <c r="I191" s="18"/>
+      <c r="D191" s="17"/>
+      <c r="E191" s="17"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="17"/>
+      <c r="H191" s="17"/>
+      <c r="I191" s="17"/>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
@@ -4067,12 +4064,12 @@
       </c>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
-      <c r="D192" s="18"/>
-      <c r="E192" s="18"/>
-      <c r="F192" s="18"/>
-      <c r="G192" s="18"/>
-      <c r="H192" s="18"/>
-      <c r="I192" s="18"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="17"/>
+      <c r="G192" s="17"/>
+      <c r="H192" s="17"/>
+      <c r="I192" s="17"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
@@ -4081,12 +4078,12 @@
       </c>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
-      <c r="D193" s="18"/>
-      <c r="E193" s="18"/>
-      <c r="F193" s="18"/>
-      <c r="G193" s="18"/>
-      <c r="H193" s="18"/>
-      <c r="I193" s="18"/>
+      <c r="D193" s="17"/>
+      <c r="E193" s="17"/>
+      <c r="F193" s="17"/>
+      <c r="G193" s="17"/>
+      <c r="H193" s="17"/>
+      <c r="I193" s="17"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
@@ -4095,12 +4092,12 @@
       </c>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
-      <c r="D194" s="19"/>
-      <c r="E194" s="18"/>
-      <c r="F194" s="18"/>
-      <c r="G194" s="18"/>
-      <c r="H194" s="18"/>
-      <c r="I194" s="18"/>
+      <c r="D194" s="18"/>
+      <c r="E194" s="17"/>
+      <c r="F194" s="17"/>
+      <c r="G194" s="17"/>
+      <c r="H194" s="17"/>
+      <c r="I194" s="17"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
@@ -4109,12 +4106,12 @@
       </c>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
-      <c r="D195" s="19"/>
-      <c r="E195" s="18"/>
-      <c r="F195" s="18"/>
-      <c r="G195" s="18"/>
-      <c r="H195" s="18"/>
-      <c r="I195" s="18"/>
+      <c r="D195" s="18"/>
+      <c r="E195" s="17"/>
+      <c r="F195" s="17"/>
+      <c r="G195" s="17"/>
+      <c r="H195" s="17"/>
+      <c r="I195" s="17"/>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
@@ -4123,12 +4120,12 @@
       </c>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
-      <c r="D196" s="19"/>
-      <c r="E196" s="18"/>
-      <c r="F196" s="18"/>
-      <c r="G196" s="18"/>
-      <c r="H196" s="18"/>
-      <c r="I196" s="18"/>
+      <c r="D196" s="18"/>
+      <c r="E196" s="17"/>
+      <c r="F196" s="17"/>
+      <c r="G196" s="17"/>
+      <c r="H196" s="17"/>
+      <c r="I196" s="17"/>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="9">
@@ -4137,37 +4134,42 @@
       </c>
       <c r="B197" s="10"/>
       <c r="C197" s="10"/>
-      <c r="D197" s="20"/>
-      <c r="E197" s="18"/>
-      <c r="F197" s="18"/>
-      <c r="G197" s="18"/>
-      <c r="H197" s="18"/>
-      <c r="I197" s="18"/>
+      <c r="D197" s="19"/>
+      <c r="E197" s="17"/>
+      <c r="F197" s="17"/>
+      <c r="G197" s="17"/>
+      <c r="H197" s="17"/>
+      <c r="I197" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:I197">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>OR($C5="Select_Dropdown",$C5="Radio_Button")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>OR($C5="Browser_Back",$C5="Browser_Forward",$C5="Browser_Refresh",$C5="Capture_Alert",$C5="Admin_Portal_Login",$C5="Browser_Quit",$C5="SINT_Login")</formula>
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>OR($C5="Browser_Back",$C5="Browser_Forward",$C5="Browser_Refresh",$C5="Capture_Alert",$C5="Browser_Quit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197 D5:F197">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>OR($C5="Check_Box_Data",$C5="Check_Log_File",$C5="Write_Box_Data")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I197 D5:E197">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>OR($C5="Click_Button",$C5="Check_Box",$C5="List_All_Dropdown_Values")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D197 H5:I197">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>OR($C5="Portal_Login",$C5="Handle_Browser_window",$C5="Ping_Test",$C5="Open_URL",$C5="Check_URL",$C5="iPause",$C5="Check_Screen_Data",$C5="Execute_System_Command",$C5="Check_Browser_Title",$C5="Send_Special_keys")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D197 F5:F197 H5:I197">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>OR($C5="Login")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4192,7 +4194,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$2:$A$26</xm:f>
+            <xm:f>Lists!$A$2:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C197</xm:sqref>
         </x14:dataValidation>
@@ -4204,10 +4206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4219,14 +4221,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="16"/>
       <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4235,7 +4237,7 @@
       </c>
       <c r="B2" s="12"/>
       <c r="D2" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4244,25 +4246,25 @@
       </c>
       <c r="B3" s="12"/>
       <c r="D3" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
+      <c r="A4" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="12"/>
       <c r="D4" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>9</v>
+      <c r="A5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="13"/>
       <c r="D5" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4273,34 +4275,34 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="13"/>
       <c r="D7" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="13"/>
       <c r="D8" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="13"/>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4309,7 +4311,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4318,7 +4320,7 @@
       </c>
       <c r="B11" s="13"/>
       <c r="D11" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4327,7 +4329,7 @@
       </c>
       <c r="B12" s="13"/>
       <c r="D12" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4336,25 +4338,25 @@
       </c>
       <c r="B13" s="13"/>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="13"/>
       <c r="D14" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="13"/>
       <c r="D15" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4371,63 +4373,45 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B18" s="13"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="13"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="13"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>34</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B24" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>